<commit_message>
fix(orders): correct Excel export data mapping and add smart aggregation for all header fields
</commit_message>
<xml_diff>
--- a/public/templates/order_template.xlsx
+++ b/public/templates/order_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\CNC_Milling\WORK_CNC\SOFT\ProjectDB\CRM\UI_ERP\React-Admin\front_Refine_v1\ai_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\CNC_Milling\WORK_CNC\SOFT\ProjectDB\CRM\UI_ERP\React-Admin\front_Refine_v1\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D83998D-D091-4437-90C2-A5DD8A79FD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACA8697-3FE6-4355-AAA9-478E20F31F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25770" yWindow="345" windowWidth="22695" windowHeight="20670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2715" yWindow="1845" windowWidth="16110" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заказ" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,10 @@
   </sheets>
   <definedNames>
     <definedName name="МДФ">Заказ!$AK$83:$AK$87</definedName>
-    <definedName name="обкат">Таблица2[Обкат]</definedName>
+    <definedName name="обкат">Списки!$C$2:$C$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Заказ!$A$1:$M$67</definedName>
-    <definedName name="пленка">Таблица3[Пленка]</definedName>
-    <definedName name="тип_детали">Таблица1[Тип детали]</definedName>
+    <definedName name="пленка">Списки!$E$2:$E$34</definedName>
+    <definedName name="тип_детали">Списки!$A$2:$A$28</definedName>
     <definedName name="фасад">Заказ!$AI$1:$AJ$5</definedName>
     <definedName name="фрезеровка">Заказ!$A$5</definedName>
     <definedName name="цена_кв_м">#REF!</definedName>
@@ -831,7 +831,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -906,14 +906,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1049,8 +1043,167 @@
     <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1058,164 +1211,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1224,232 +1221,7 @@
     <cellStyle name="Процентный" xfId="3" builtinId="5"/>
     <cellStyle name="Финансовый" xfId="2" builtinId="3"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1460,36 +1232,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A1:A28" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A1:A28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Тип детали" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Таблица2" displayName="Таблица2" ref="C1:C5" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="C1:C5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Обкат" dataDxfId="5"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Таблица3" displayName="Таблица3" ref="E1:E34" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="E1:E34" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Пленка" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1782,8 +1524,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:AA82"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,283 +1546,283 @@
     <col min="14" max="14" width="1.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="46" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="3.7109375" style="1" customWidth="1"/>
     <col min="21" max="24" width="11.85546875" style="1" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71">
+      <c r="A1" s="69">
         <v>25</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="74" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="89" t="s">
+      <c r="E1" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="89"/>
-      <c r="L1" s="95" t="s">
+      <c r="K1" s="118"/>
+      <c r="L1" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="95"/>
-      <c r="N1" s="61"/>
-      <c r="P1" s="38" t="s">
+      <c r="M1" s="113"/>
+      <c r="N1" s="59"/>
+      <c r="P1" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="57" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="128" t="s">
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="102">
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="120">
         <f>SUM(J12:J52)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="102"/>
-      <c r="L2" s="101">
+      <c r="K2" s="120"/>
+      <c r="L2" s="119">
         <f>J2-(J2*P2)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="101"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
     </row>
     <row r="3" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="50"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="78" t="s">
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="48"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" s="79"/>
-      <c r="AA3" s="79"/>
+      <c r="Z3" s="130"/>
+      <c r="AA3" s="130"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="105" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="87" t="s">
+      <c r="E4" s="92"/>
+      <c r="F4" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="98" t="s">
+      <c r="G4" s="103"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="99">
+      <c r="K4" s="116">
         <f>IF(ISBLANK(L2), (J2-SUM(Q6:Q42)), (L2-SUM(Q6:Q42)))</f>
         <v>0</v>
       </c>
-      <c r="L4" s="99"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="40"/>
+      <c r="L4" s="116"/>
+      <c r="M4" s="117"/>
+      <c r="N4" s="38"/>
       <c r="O4" s="85" t="s">
         <v>96</v>
       </c>
       <c r="P4" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="Q4" s="103" t="s">
+      <c r="Q4" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="79"/>
-      <c r="AA4" s="79"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="129"/>
+      <c r="Z4" s="130"/>
+      <c r="AA4" s="130"/>
     </row>
     <row r="5" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="108"/>
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="117"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="40"/>
+      <c r="A5" s="93"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="38"/>
       <c r="O5" s="86"/>
       <c r="P5" s="86"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="36">
+      <c r="Q5" s="87"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
+      <c r="Y5" s="34">
         <f>IF(F12="выборка",1,IF(F12="выборка-2ступени",2,0))</f>
         <v>0</v>
       </c>
-      <c r="Z5" s="35"/>
+      <c r="Z5" s="33"/>
     </row>
     <row r="6" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="109"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="117"/>
-      <c r="J6" s="98" t="s">
+      <c r="A6" s="94"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="104"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="104"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
     </row>
     <row r="7" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="109"/>
-      <c r="B7" s="109"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
+      <c r="A7" s="94"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
     </row>
     <row r="8" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="110" t="s">
+      <c r="A8" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="111"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="114"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="100"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="91" t="s">
+      <c r="H8" s="125"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="124">
+      <c r="K8" s="111">
         <f>SUM(E12:E52)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="91" t="s">
+      <c r="L8" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="93">
+      <c r="M8" s="122">
         <f>SUM(D12:D52)</f>
         <v>0</v>
       </c>
       <c r="N8" s="14"/>
-      <c r="O8" s="66"/>
+      <c r="O8" s="64"/>
       <c r="P8" s="8"/>
-      <c r="Q8" s="47"/>
+      <c r="Q8" s="45"/>
       <c r="R8" s="14"/>
       <c r="S8" s="14"/>
       <c r="T8" s="14"/>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="117"/>
-      <c r="D9" s="117"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="115"/>
+      <c r="A9" s="98"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="101"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="125"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="94"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="123"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="66"/>
+      <c r="O9" s="64"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="47"/>
+      <c r="Q9" s="45"/>
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
-      <c r="U9" s="89" t="s">
+      <c r="U9" s="118" t="s">
         <v>80</v>
       </c>
       <c r="V9" s="1" t="s">
@@ -2103,13 +1845,13 @@
       <c r="L10" s="12"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
-      <c r="O10" s="66"/>
+      <c r="O10" s="64"/>
       <c r="P10" s="8"/>
-      <c r="Q10" s="47"/>
+      <c r="Q10" s="45"/>
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
-      <c r="U10" s="89"/>
+      <c r="U10" s="118"/>
     </row>
     <row r="11" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -2130,10 +1872,10 @@
       <c r="F11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="73" t="s">
+      <c r="G11" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="72" t="s">
+      <c r="H11" s="70" t="s">
         <v>98</v>
       </c>
       <c r="I11" s="18" t="s">
@@ -2142,33 +1884,33 @@
       <c r="J11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="90" t="s">
+      <c r="K11" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="38">
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="36">
         <f>IF(F11="выборка",(60),IF(F11="выборка-2ступени",(67),0))</f>
         <v>0</v>
       </c>
-      <c r="V11" s="38" t="s">
+      <c r="V11" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="W11" s="38" t="s">
+      <c r="W11" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38" t="s">
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="Z11" s="38" t="s">
+      <c r="Z11" s="36" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2176,10 +1918,10 @@
       <c r="A12" s="8">
         <v>1</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="76">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="74">
         <f>ROUNDUP((B12/1000)*(C12/1000)*D12,2)</f>
         <v>0</v>
       </c>
@@ -2191,37 +1933,37 @@
         <f t="shared" ref="J12:J42" si="0">E12*I12</f>
         <v>0</v>
       </c>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
+      <c r="K12" s="88"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="88"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="69"/>
+      <c r="O12" s="67"/>
       <c r="P12" s="8"/>
-      <c r="Q12" s="47"/>
+      <c r="Q12" s="45"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="19">
         <f>IF(F12="выборка",(60),IF(F12="выборка-2ступени",(67),0))</f>
         <v>0</v>
       </c>
-      <c r="U12" s="38">
+      <c r="U12" s="36">
         <f t="shared" ref="U12:U20" si="1">IF(F12="выборка",(60),IF(F12="выборка-2ступени",(67),0))</f>
         <v>0</v>
       </c>
-      <c r="V12" s="38">
+      <c r="V12" s="36">
         <f>IF(AND((B12 - U12*2-1)&gt;0,U12&gt;0),B12 - U12*2-1,0)</f>
         <v>0</v>
       </c>
-      <c r="W12" s="38">
+      <c r="W12" s="36">
         <f>IF(AND((C12 - U12*2-1)&gt;0,U12&gt;0),C12 - U12*2-1,0)</f>
         <v>0</v>
       </c>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38">
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36">
         <f>IF(F12="выборка",(B12 - 60*2-1),IF(F12="выборка-2ступени",(B12 - 67*2-1),0))</f>
         <v>0</v>
       </c>
-      <c r="Z12" s="38">
+      <c r="Z12" s="36">
         <f>IF(F12="выборка",(C12 - 60*2-1),IF(F12="выборка-2ступени",(C12 - 67*2-1),0))</f>
         <v>0</v>
       </c>
@@ -2230,9 +1972,9 @@
       <c r="A13" s="8">
         <v>2</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="20">
         <f t="shared" ref="E13:E42" si="2">ROUNDUP((B13/1000)*(C13/1000)*D13,2)</f>
         <v>0</v>
@@ -2245,34 +1987,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="77"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="77"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="88"/>
+      <c r="M13" s="88"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="69"/>
+      <c r="O13" s="67"/>
       <c r="P13" s="8"/>
-      <c r="Q13" s="47"/>
+      <c r="Q13" s="45"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="19"/>
-      <c r="U13" s="38">
+      <c r="U13" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V13" s="38">
+      <c r="V13" s="36">
         <f t="shared" ref="V13:V42" si="3">IF(AND((B13 - U13*2-1)&gt;0,U13&gt;0),B13 - U13*2-1,0)</f>
         <v>0</v>
       </c>
-      <c r="W13" s="38">
+      <c r="W13" s="36">
         <f t="shared" ref="W13:W42" si="4">IF(AND((C13 - U13*2-1)&gt;0,U13&gt;0),C13 - U13*2-1,0)</f>
         <v>0</v>
       </c>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="38">
+      <c r="X13" s="36"/>
+      <c r="Y13" s="36">
         <f t="shared" ref="Y13:Y42" si="5">IF(F13="выборка",(B13 - 60*2-1),IF(F13="выборка-2ступени",(B13 - 67*2-1),0))</f>
         <v>0</v>
       </c>
-      <c r="Z13" s="38">
+      <c r="Z13" s="36">
         <f t="shared" ref="Z13:Z42" si="6">IF(F13="выборка",(C13 - 60*2-1),IF(F13="выборка-2ступени",(C13 - 67*2-1),0))</f>
         <v>0</v>
       </c>
@@ -2281,9 +2023,9 @@
       <c r="A14" s="8">
         <v>3</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2296,34 +2038,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
       <c r="N14" s="5"/>
-      <c r="O14" s="69"/>
+      <c r="O14" s="67"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="47"/>
+      <c r="Q14" s="45"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="19"/>
-      <c r="U14" s="38">
+      <c r="U14" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V14" s="38">
+      <c r="V14" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W14" s="38">
+      <c r="W14" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38">
+      <c r="X14" s="36"/>
+      <c r="Y14" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z14" s="38">
+      <c r="Z14" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2332,9 +2074,9 @@
       <c r="A15" s="8">
         <v>4</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2347,34 +2089,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="77"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="53"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="51"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="19"/>
-      <c r="U15" s="38">
+      <c r="U15" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V15" s="38">
+      <c r="V15" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W15" s="38">
+      <c r="W15" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="38">
+      <c r="X15" s="36"/>
+      <c r="Y15" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z15" s="38">
+      <c r="Z15" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2383,9 +2125,9 @@
       <c r="A16" s="8">
         <v>5</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
       <c r="E16" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2398,34 +2140,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="77"/>
-      <c r="L16" s="77"/>
-      <c r="M16" s="77"/>
+      <c r="K16" s="88"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="88"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="52"/>
-      <c r="Q16" s="53"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="51"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="19"/>
-      <c r="U16" s="38">
+      <c r="U16" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V16" s="38">
+      <c r="V16" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W16" s="38">
+      <c r="W16" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="38">
+      <c r="X16" s="36"/>
+      <c r="Y16" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z16" s="38">
+      <c r="Z16" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2434,9 +2176,9 @@
       <c r="A17" s="8">
         <v>6</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
       <c r="E17" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2449,34 +2191,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K17" s="77"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="77"/>
+      <c r="K17" s="88"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="88"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="53"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="51"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="19"/>
-      <c r="U17" s="38">
+      <c r="U17" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V17" s="38">
+      <c r="V17" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W17" s="38">
+      <c r="W17" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38">
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z17" s="38">
+      <c r="Z17" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2485,9 +2227,9 @@
       <c r="A18" s="8">
         <v>7</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2500,34 +2242,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="77"/>
-      <c r="L18" s="77"/>
-      <c r="M18" s="77"/>
+      <c r="K18" s="88"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="53"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="51"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="19"/>
-      <c r="U18" s="38">
+      <c r="U18" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V18" s="38">
+      <c r="V18" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W18" s="38">
+      <c r="W18" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="38">
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z18" s="38">
+      <c r="Z18" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2536,9 +2278,9 @@
       <c r="A19" s="8">
         <v>8</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
       <c r="E19" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2551,34 +2293,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K19" s="77"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
+      <c r="K19" s="88"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="52"/>
-      <c r="Q19" s="53"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="51"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="19"/>
-      <c r="U19" s="38">
+      <c r="U19" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V19" s="38">
+      <c r="V19" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W19" s="38">
+      <c r="W19" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38">
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z19" s="38">
+      <c r="Z19" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2587,9 +2329,9 @@
       <c r="A20" s="8">
         <v>9</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
       <c r="E20" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2602,34 +2344,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="77"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="77"/>
+      <c r="K20" s="88"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="88"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
-      <c r="P20" s="52"/>
-      <c r="Q20" s="53"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="51"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="19"/>
-      <c r="U20" s="38">
+      <c r="U20" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V20" s="38">
+      <c r="V20" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W20" s="38">
+      <c r="W20" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="38">
+      <c r="X20" s="36"/>
+      <c r="Y20" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z20" s="38">
+      <c r="Z20" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2638,9 +2380,9 @@
       <c r="A21" s="8">
         <v>10</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
       <c r="E21" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2653,34 +2395,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="77"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-      <c r="P21" s="52"/>
-      <c r="Q21" s="53"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="51"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="19"/>
-      <c r="U21" s="38">
+      <c r="U21" s="36">
         <f t="shared" ref="U21:U42" si="7">IF(F21="выборка",(60),IF(F21="выборка-2ступени",(67),0))</f>
         <v>0</v>
       </c>
-      <c r="V21" s="38">
+      <c r="V21" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W21" s="38">
+      <c r="W21" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X21" s="38"/>
-      <c r="Y21" s="38">
+      <c r="X21" s="36"/>
+      <c r="Y21" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z21" s="38">
+      <c r="Z21" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2689,9 +2431,9 @@
       <c r="A22" s="8">
         <v>11</v>
       </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2704,34 +2446,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="77"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="77"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="88"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="52"/>
-      <c r="Q22" s="53"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="51"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="19"/>
-      <c r="U22" s="38">
+      <c r="U22" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V22" s="38">
+      <c r="V22" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W22" s="38">
+      <c r="W22" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X22" s="38"/>
-      <c r="Y22" s="38">
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z22" s="38">
+      <c r="Z22" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2740,9 +2482,9 @@
       <c r="A23" s="8">
         <v>12</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2755,34 +2497,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
+      <c r="K23" s="88"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="88"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="53"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="51"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="19"/>
-      <c r="U23" s="38">
+      <c r="U23" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V23" s="38">
+      <c r="V23" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W23" s="38">
+      <c r="W23" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X23" s="38"/>
-      <c r="Y23" s="38">
+      <c r="X23" s="36"/>
+      <c r="Y23" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z23" s="38">
+      <c r="Z23" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2791,9 +2533,9 @@
       <c r="A24" s="8">
         <v>13</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
       <c r="E24" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2806,34 +2548,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="77"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="53"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="51"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="19"/>
-      <c r="U24" s="38">
+      <c r="U24" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V24" s="38">
+      <c r="V24" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W24" s="38">
+      <c r="W24" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38">
+      <c r="X24" s="36"/>
+      <c r="Y24" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z24" s="38">
+      <c r="Z24" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2842,9 +2584,9 @@
       <c r="A25" s="8">
         <v>14</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2857,34 +2599,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="88"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-      <c r="P25" s="52"/>
-      <c r="Q25" s="53"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="51"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="19"/>
-      <c r="U25" s="38">
+      <c r="U25" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V25" s="38">
+      <c r="V25" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W25" s="38">
+      <c r="W25" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38">
+      <c r="X25" s="36"/>
+      <c r="Y25" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z25" s="38">
+      <c r="Z25" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2893,9 +2635,9 @@
       <c r="A26" s="8">
         <v>15</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2908,34 +2650,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="88"/>
+      <c r="M26" s="88"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-      <c r="P26" s="52"/>
-      <c r="Q26" s="53"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="51"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
       <c r="T26" s="19"/>
-      <c r="U26" s="38">
+      <c r="U26" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V26" s="38">
+      <c r="V26" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W26" s="38">
+      <c r="W26" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="38">
+      <c r="X26" s="36"/>
+      <c r="Y26" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z26" s="38">
+      <c r="Z26" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2944,9 +2686,9 @@
       <c r="A27" s="8">
         <v>16</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2959,34 +2701,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="77"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="88"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
-      <c r="P27" s="52"/>
-      <c r="Q27" s="53"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="51"/>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="19"/>
-      <c r="U27" s="38">
+      <c r="U27" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V27" s="38">
+      <c r="V27" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W27" s="38">
+      <c r="W27" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38">
+      <c r="X27" s="36"/>
+      <c r="Y27" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z27" s="38">
+      <c r="Z27" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2995,9 +2737,9 @@
       <c r="A28" s="8">
         <v>17</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
       <c r="E28" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3010,34 +2752,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K28" s="77"/>
-      <c r="L28" s="77"/>
-      <c r="M28" s="80"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="88"/>
+      <c r="M28" s="124"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
-      <c r="P28" s="52"/>
-      <c r="Q28" s="53"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="51"/>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
       <c r="T28" s="19"/>
-      <c r="U28" s="38">
+      <c r="U28" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V28" s="38">
+      <c r="V28" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W28" s="38">
+      <c r="W28" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X28" s="38"/>
-      <c r="Y28" s="38">
+      <c r="X28" s="36"/>
+      <c r="Y28" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z28" s="38">
+      <c r="Z28" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3046,9 +2788,9 @@
       <c r="A29" s="8">
         <v>18</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
       <c r="E29" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3061,34 +2803,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="77"/>
-      <c r="L29" s="77"/>
-      <c r="M29" s="80"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="88"/>
+      <c r="M29" s="124"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
-      <c r="P29" s="52"/>
-      <c r="Q29" s="53"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="51"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="19"/>
-      <c r="U29" s="38">
+      <c r="U29" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V29" s="38">
+      <c r="V29" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W29" s="38">
+      <c r="W29" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X29" s="38"/>
-      <c r="Y29" s="38">
+      <c r="X29" s="36"/>
+      <c r="Y29" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z29" s="38">
+      <c r="Z29" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3097,9 +2839,9 @@
       <c r="A30" s="8">
         <v>19</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
       <c r="E30" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3112,34 +2854,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K30" s="77"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="80"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="124"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
-      <c r="P30" s="52"/>
-      <c r="Q30" s="53"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="51"/>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="19"/>
-      <c r="U30" s="38">
+      <c r="U30" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V30" s="38">
+      <c r="V30" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W30" s="38">
+      <c r="W30" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X30" s="38"/>
-      <c r="Y30" s="38">
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z30" s="38">
+      <c r="Z30" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3148,9 +2890,9 @@
       <c r="A31" s="8">
         <v>20</v>
       </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3163,34 +2905,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="80"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="88"/>
+      <c r="M31" s="124"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="53"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="51"/>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="19"/>
-      <c r="U31" s="38">
+      <c r="U31" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V31" s="38">
+      <c r="V31" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W31" s="38">
+      <c r="W31" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X31" s="38"/>
-      <c r="Y31" s="38">
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z31" s="38">
+      <c r="Z31" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3199,9 +2941,9 @@
       <c r="A32" s="8">
         <v>21</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3214,34 +2956,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="77"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="88"/>
+      <c r="M32" s="88"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="53"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="51"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="19"/>
-      <c r="U32" s="38">
+      <c r="U32" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V32" s="38">
+      <c r="V32" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W32" s="38">
+      <c r="W32" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X32" s="38"/>
-      <c r="Y32" s="38">
+      <c r="X32" s="36"/>
+      <c r="Y32" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z32" s="38">
+      <c r="Z32" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3250,9 +2992,9 @@
       <c r="A33" s="8">
         <v>22</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3265,34 +3007,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="M33" s="88"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="53"/>
+      <c r="P33" s="50"/>
+      <c r="Q33" s="51"/>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="19"/>
-      <c r="U33" s="38">
+      <c r="U33" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V33" s="38">
+      <c r="V33" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W33" s="38">
+      <c r="W33" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X33" s="38"/>
-      <c r="Y33" s="38">
+      <c r="X33" s="36"/>
+      <c r="Y33" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z33" s="38">
+      <c r="Z33" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3301,9 +3043,9 @@
       <c r="A34" s="8">
         <v>23</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3316,34 +3058,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
+      <c r="K34" s="88"/>
+      <c r="L34" s="88"/>
+      <c r="M34" s="88"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="53"/>
+      <c r="P34" s="50"/>
+      <c r="Q34" s="51"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="19"/>
-      <c r="U34" s="38">
+      <c r="U34" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V34" s="38">
+      <c r="V34" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W34" s="38">
+      <c r="W34" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X34" s="38"/>
-      <c r="Y34" s="38">
+      <c r="X34" s="36"/>
+      <c r="Y34" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z34" s="38">
+      <c r="Z34" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3352,9 +3094,9 @@
       <c r="A35" s="8">
         <v>24</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
       <c r="E35" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3367,34 +3109,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="77"/>
-      <c r="L35" s="77"/>
-      <c r="M35" s="77"/>
+      <c r="K35" s="88"/>
+      <c r="L35" s="88"/>
+      <c r="M35" s="88"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="53"/>
+      <c r="P35" s="50"/>
+      <c r="Q35" s="51"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="19"/>
-      <c r="U35" s="38">
+      <c r="U35" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V35" s="38">
+      <c r="V35" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W35" s="38">
+      <c r="W35" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X35" s="38"/>
-      <c r="Y35" s="38">
+      <c r="X35" s="36"/>
+      <c r="Y35" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z35" s="38">
+      <c r="Z35" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3403,9 +3145,9 @@
       <c r="A36" s="8">
         <v>25</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
       <c r="E36" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3418,34 +3160,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K36" s="77"/>
-      <c r="L36" s="77"/>
-      <c r="M36" s="77"/>
+      <c r="K36" s="88"/>
+      <c r="L36" s="88"/>
+      <c r="M36" s="88"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
-      <c r="P36" s="52"/>
-      <c r="Q36" s="53"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="51"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
       <c r="T36" s="19"/>
-      <c r="U36" s="38">
+      <c r="U36" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V36" s="38">
+      <c r="V36" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W36" s="38">
+      <c r="W36" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X36" s="38"/>
-      <c r="Y36" s="38">
+      <c r="X36" s="36"/>
+      <c r="Y36" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z36" s="38">
+      <c r="Z36" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3454,9 +3196,9 @@
       <c r="A37" s="8">
         <v>26</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
       <c r="E37" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3469,34 +3211,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="77"/>
-      <c r="L37" s="77"/>
-      <c r="M37" s="77"/>
+      <c r="K37" s="88"/>
+      <c r="L37" s="88"/>
+      <c r="M37" s="88"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
-      <c r="P37" s="52"/>
-      <c r="Q37" s="53"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="51"/>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
       <c r="T37" s="19"/>
-      <c r="U37" s="38">
+      <c r="U37" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V37" s="38">
+      <c r="V37" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W37" s="38">
+      <c r="W37" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X37" s="38"/>
-      <c r="Y37" s="38">
+      <c r="X37" s="36"/>
+      <c r="Y37" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z37" s="38">
+      <c r="Z37" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3505,9 +3247,9 @@
       <c r="A38" s="8">
         <v>27</v>
       </c>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
       <c r="E38" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3520,34 +3262,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="77"/>
+      <c r="K38" s="88"/>
+      <c r="L38" s="88"/>
+      <c r="M38" s="88"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
-      <c r="P38" s="52"/>
-      <c r="Q38" s="53"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="51"/>
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
       <c r="T38" s="19"/>
-      <c r="U38" s="38">
+      <c r="U38" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V38" s="38">
+      <c r="V38" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W38" s="38">
+      <c r="W38" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X38" s="38"/>
-      <c r="Y38" s="38">
+      <c r="X38" s="36"/>
+      <c r="Y38" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z38" s="38">
+      <c r="Z38" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3556,9 +3298,9 @@
       <c r="A39" s="8">
         <v>28</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3571,34 +3313,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K39" s="77"/>
-      <c r="L39" s="77"/>
-      <c r="M39" s="77"/>
+      <c r="K39" s="88"/>
+      <c r="L39" s="88"/>
+      <c r="M39" s="88"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="53"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="51"/>
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
       <c r="T39" s="19"/>
-      <c r="U39" s="38">
+      <c r="U39" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V39" s="38">
+      <c r="V39" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W39" s="38">
+      <c r="W39" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X39" s="38"/>
-      <c r="Y39" s="38">
+      <c r="X39" s="36"/>
+      <c r="Y39" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z39" s="38">
+      <c r="Z39" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3607,9 +3349,9 @@
       <c r="A40" s="8">
         <v>29</v>
       </c>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
       <c r="E40" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3622,34 +3364,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K40" s="77"/>
-      <c r="L40" s="77"/>
-      <c r="M40" s="77"/>
+      <c r="K40" s="88"/>
+      <c r="L40" s="88"/>
+      <c r="M40" s="88"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="53"/>
+      <c r="P40" s="50"/>
+      <c r="Q40" s="51"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="19"/>
-      <c r="U40" s="38">
+      <c r="U40" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V40" s="38">
+      <c r="V40" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W40" s="38">
+      <c r="W40" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X40" s="38"/>
-      <c r="Y40" s="38">
+      <c r="X40" s="36"/>
+      <c r="Y40" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z40" s="38">
+      <c r="Z40" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3658,9 +3400,9 @@
       <c r="A41" s="8">
         <v>30</v>
       </c>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
       <c r="E41" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3673,34 +3415,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K41" s="77"/>
-      <c r="L41" s="77"/>
-      <c r="M41" s="77"/>
+      <c r="K41" s="88"/>
+      <c r="L41" s="88"/>
+      <c r="M41" s="88"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
-      <c r="P41" s="52"/>
-      <c r="Q41" s="53"/>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="51"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="19"/>
-      <c r="U41" s="38">
+      <c r="U41" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V41" s="38">
+      <c r="V41" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W41" s="38">
+      <c r="W41" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X41" s="38"/>
-      <c r="Y41" s="38">
+      <c r="X41" s="36"/>
+      <c r="Y41" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z41" s="38">
+      <c r="Z41" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3709,9 +3451,9 @@
       <c r="A42" s="8">
         <v>31</v>
       </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
       <c r="E42" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3724,34 +3466,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K42" s="77"/>
-      <c r="L42" s="77"/>
-      <c r="M42" s="77"/>
+      <c r="K42" s="88"/>
+      <c r="L42" s="88"/>
+      <c r="M42" s="88"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="53"/>
+      <c r="P42" s="50"/>
+      <c r="Q42" s="51"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
       <c r="T42" s="19"/>
-      <c r="U42" s="38">
+      <c r="U42" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V42" s="38">
+      <c r="V42" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W42" s="38">
+      <c r="W42" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X42" s="38"/>
-      <c r="Y42" s="38">
+      <c r="X42" s="36"/>
+      <c r="Y42" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z42" s="38">
+      <c r="Z42" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3760,9 +3502,9 @@
       <c r="A43" s="8">
         <v>32</v>
       </c>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
       <c r="E43" s="20">
         <f t="shared" ref="E43:E51" si="8">ROUNDUP((B43/1000)*(C43/1000)*D43,2)</f>
         <v>0</v>
@@ -3775,34 +3517,34 @@
         <f t="shared" ref="J43:J51" si="9">E43*I43</f>
         <v>0</v>
       </c>
-      <c r="K43" s="77"/>
-      <c r="L43" s="77"/>
-      <c r="M43" s="77"/>
+      <c r="K43" s="88"/>
+      <c r="L43" s="88"/>
+      <c r="M43" s="88"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
-      <c r="P43" s="52"/>
-      <c r="Q43" s="53"/>
+      <c r="P43" s="50"/>
+      <c r="Q43" s="51"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
       <c r="T43" s="19"/>
-      <c r="U43" s="38">
+      <c r="U43" s="36">
         <f t="shared" ref="U43:U52" si="10">IF(F43="выборка",(60),IF(F43="выборка-2ступени",(67),0))</f>
         <v>0</v>
       </c>
-      <c r="V43" s="38">
+      <c r="V43" s="36">
         <f t="shared" ref="V43:V52" si="11">IF(AND((B43 - U43*2-1)&gt;0,U43&gt;0),B43 - U43*2-1,0)</f>
         <v>0</v>
       </c>
-      <c r="W43" s="38">
+      <c r="W43" s="36">
         <f t="shared" ref="W43:W52" si="12">IF(AND((C43 - U43*2-1)&gt;0,U43&gt;0),C43 - U43*2-1,0)</f>
         <v>0</v>
       </c>
-      <c r="X43" s="38"/>
-      <c r="Y43" s="38">
+      <c r="X43" s="36"/>
+      <c r="Y43" s="36">
         <f t="shared" ref="Y43:Y52" si="13">IF(F43="выборка",(B43 - 60*2-1),IF(F43="выборка-2ступени",(B43 - 67*2-1),0))</f>
         <v>0</v>
       </c>
-      <c r="Z43" s="38">
+      <c r="Z43" s="36">
         <f t="shared" ref="Z43:Z52" si="14">IF(F43="выборка",(C43 - 60*2-1),IF(F43="выборка-2ступени",(C43 - 67*2-1),0))</f>
         <v>0</v>
       </c>
@@ -3811,9 +3553,9 @@
       <c r="A44" s="8">
         <v>33</v>
       </c>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
       <c r="E44" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3826,34 +3568,34 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K44" s="77"/>
-      <c r="L44" s="77"/>
-      <c r="M44" s="77"/>
+      <c r="K44" s="88"/>
+      <c r="L44" s="88"/>
+      <c r="M44" s="88"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
-      <c r="P44" s="52"/>
-      <c r="Q44" s="53"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="51"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5"/>
       <c r="T44" s="19"/>
-      <c r="U44" s="38">
+      <c r="U44" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V44" s="38">
+      <c r="V44" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W44" s="38">
+      <c r="W44" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X44" s="38"/>
-      <c r="Y44" s="38">
+      <c r="X44" s="36"/>
+      <c r="Y44" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z44" s="38">
+      <c r="Z44" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -3862,9 +3604,9 @@
       <c r="A45" s="8">
         <v>34</v>
       </c>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
       <c r="E45" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3877,34 +3619,34 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K45" s="77"/>
-      <c r="L45" s="77"/>
-      <c r="M45" s="77"/>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="88"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
-      <c r="P45" s="52"/>
-      <c r="Q45" s="53"/>
+      <c r="P45" s="50"/>
+      <c r="Q45" s="51"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
       <c r="T45" s="19"/>
-      <c r="U45" s="38">
+      <c r="U45" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V45" s="38">
+      <c r="V45" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W45" s="38">
+      <c r="W45" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X45" s="38"/>
-      <c r="Y45" s="38">
+      <c r="X45" s="36"/>
+      <c r="Y45" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z45" s="38">
+      <c r="Z45" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -3913,9 +3655,9 @@
       <c r="A46" s="8">
         <v>35</v>
       </c>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
       <c r="E46" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3928,34 +3670,34 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K46" s="77"/>
-      <c r="L46" s="77"/>
-      <c r="M46" s="77"/>
+      <c r="K46" s="88"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="88"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
-      <c r="P46" s="52"/>
-      <c r="Q46" s="53"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="51"/>
       <c r="R46" s="5"/>
       <c r="S46" s="5"/>
       <c r="T46" s="19"/>
-      <c r="U46" s="38">
+      <c r="U46" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V46" s="38">
+      <c r="V46" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W46" s="38">
+      <c r="W46" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X46" s="38"/>
-      <c r="Y46" s="38">
+      <c r="X46" s="36"/>
+      <c r="Y46" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z46" s="38">
+      <c r="Z46" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -3964,9 +3706,9 @@
       <c r="A47" s="8">
         <v>36</v>
       </c>
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
       <c r="E47" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3979,34 +3721,34 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K47" s="77"/>
-      <c r="L47" s="77"/>
-      <c r="M47" s="77"/>
+      <c r="K47" s="88"/>
+      <c r="L47" s="88"/>
+      <c r="M47" s="88"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
-      <c r="P47" s="52"/>
-      <c r="Q47" s="53"/>
+      <c r="P47" s="50"/>
+      <c r="Q47" s="51"/>
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
       <c r="T47" s="19"/>
-      <c r="U47" s="38">
+      <c r="U47" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V47" s="38">
+      <c r="V47" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W47" s="38">
+      <c r="W47" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X47" s="38"/>
-      <c r="Y47" s="38">
+      <c r="X47" s="36"/>
+      <c r="Y47" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z47" s="38">
+      <c r="Z47" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -4015,9 +3757,9 @@
       <c r="A48" s="8">
         <v>37</v>
       </c>
-      <c r="B48" s="44"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
       <c r="E48" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4030,34 +3772,34 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K48" s="77"/>
-      <c r="L48" s="77"/>
-      <c r="M48" s="77"/>
+      <c r="K48" s="88"/>
+      <c r="L48" s="88"/>
+      <c r="M48" s="88"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
-      <c r="P48" s="52"/>
-      <c r="Q48" s="53"/>
+      <c r="P48" s="50"/>
+      <c r="Q48" s="51"/>
       <c r="R48" s="5"/>
       <c r="S48" s="5"/>
       <c r="T48" s="19"/>
-      <c r="U48" s="38">
+      <c r="U48" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V48" s="38">
+      <c r="V48" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W48" s="38">
+      <c r="W48" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X48" s="38"/>
-      <c r="Y48" s="38">
+      <c r="X48" s="36"/>
+      <c r="Y48" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z48" s="38">
+      <c r="Z48" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -4066,9 +3808,9 @@
       <c r="A49" s="8">
         <v>38</v>
       </c>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
       <c r="E49" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4081,34 +3823,34 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K49" s="77"/>
-      <c r="L49" s="77"/>
-      <c r="M49" s="77"/>
+      <c r="K49" s="88"/>
+      <c r="L49" s="88"/>
+      <c r="M49" s="88"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
-      <c r="P49" s="52"/>
-      <c r="Q49" s="53"/>
+      <c r="P49" s="50"/>
+      <c r="Q49" s="51"/>
       <c r="R49" s="5"/>
       <c r="S49" s="5"/>
       <c r="T49" s="19"/>
-      <c r="U49" s="38">
+      <c r="U49" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V49" s="38">
+      <c r="V49" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W49" s="38">
+      <c r="W49" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X49" s="38"/>
-      <c r="Y49" s="38">
+      <c r="X49" s="36"/>
+      <c r="Y49" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z49" s="38">
+      <c r="Z49" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -4117,9 +3859,9 @@
       <c r="A50" s="8">
         <v>39</v>
       </c>
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
       <c r="E50" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4132,34 +3874,34 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K50" s="77"/>
-      <c r="L50" s="77"/>
-      <c r="M50" s="77"/>
+      <c r="K50" s="88"/>
+      <c r="L50" s="88"/>
+      <c r="M50" s="88"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
-      <c r="P50" s="52"/>
-      <c r="Q50" s="53"/>
+      <c r="P50" s="50"/>
+      <c r="Q50" s="51"/>
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
       <c r="T50" s="19"/>
-      <c r="U50" s="38">
+      <c r="U50" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V50" s="38">
+      <c r="V50" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W50" s="38">
+      <c r="W50" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X50" s="38"/>
-      <c r="Y50" s="38">
+      <c r="X50" s="36"/>
+      <c r="Y50" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z50" s="38">
+      <c r="Z50" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -4168,9 +3910,9 @@
       <c r="A51" s="8">
         <v>40</v>
       </c>
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="42"/>
       <c r="E51" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4183,138 +3925,138 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K51" s="77"/>
-      <c r="L51" s="77"/>
-      <c r="M51" s="77"/>
+      <c r="K51" s="88"/>
+      <c r="L51" s="88"/>
+      <c r="M51" s="88"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
-      <c r="P51" s="52"/>
-      <c r="Q51" s="53"/>
+      <c r="P51" s="50"/>
+      <c r="Q51" s="51"/>
       <c r="R51" s="5"/>
       <c r="S51" s="5"/>
       <c r="T51" s="19"/>
-      <c r="U51" s="38">
+      <c r="U51" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V51" s="38">
+      <c r="V51" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W51" s="38">
+      <c r="W51" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X51" s="38"/>
-      <c r="Y51" s="38">
+      <c r="X51" s="36"/>
+      <c r="Y51" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z51" s="38">
+      <c r="Z51" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:26" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P52" s="52"/>
-      <c r="Q52" s="54"/>
+      <c r="P52" s="50"/>
+      <c r="Q52" s="52"/>
       <c r="T52" s="19"/>
-      <c r="U52" s="38">
+      <c r="U52" s="36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V52" s="38">
+      <c r="V52" s="36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W52" s="38">
+      <c r="W52" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X52" s="38"/>
-      <c r="Y52" s="38">
+      <c r="X52" s="36"/>
+      <c r="Y52" s="36">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Z52" s="38">
+      <c r="Z52" s="36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:26" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="127" t="s">
+      <c r="A53" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="127"/>
-      <c r="C53" s="127"/>
-      <c r="D53" s="127"/>
-      <c r="E53" s="127"/>
-      <c r="F53" s="127"/>
-      <c r="G53" s="127"/>
-      <c r="H53" s="127"/>
+      <c r="B53" s="79"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="79"/>
       <c r="I53" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P53" s="52"/>
-      <c r="Q53" s="54"/>
+      <c r="P53" s="50"/>
+      <c r="Q53" s="52"/>
     </row>
     <row r="54" spans="1:26" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="127"/>
-      <c r="B54" s="127"/>
-      <c r="C54" s="127"/>
-      <c r="D54" s="127"/>
-      <c r="E54" s="127"/>
-      <c r="F54" s="127"/>
-      <c r="G54" s="127"/>
-      <c r="H54" s="127"/>
+      <c r="A54" s="79"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="79"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="79"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="79"/>
       <c r="I54" s="3"/>
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
       <c r="L54" s="7"/>
       <c r="M54" s="7"/>
-      <c r="N54" s="43"/>
-      <c r="O54" s="43"/>
-      <c r="P54" s="55"/>
-      <c r="Q54" s="56"/>
-      <c r="R54" s="43"/>
-      <c r="S54" s="43"/>
-      <c r="T54" s="43"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="41"/>
+      <c r="P54" s="53"/>
+      <c r="Q54" s="54"/>
+      <c r="R54" s="41"/>
+      <c r="S54" s="41"/>
+      <c r="T54" s="41"/>
     </row>
     <row r="55" spans="1:26" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="132" t="s">
+      <c r="A55" s="84" t="s">
         <v>103</v>
       </c>
-      <c r="B55" s="132"/>
-      <c r="C55" s="132"/>
-      <c r="D55" s="132"/>
-      <c r="E55" s="132"/>
-      <c r="F55" s="132"/>
-      <c r="G55" s="132"/>
-      <c r="H55" s="132"/>
-      <c r="I55" s="132"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="43"/>
-      <c r="N55" s="43"/>
-      <c r="O55" s="43"/>
-      <c r="P55" s="55"/>
-      <c r="Q55" s="56"/>
-      <c r="R55" s="43"/>
-      <c r="S55" s="43"/>
-      <c r="T55" s="43"/>
+      <c r="B55" s="84"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
+      <c r="F55" s="84"/>
+      <c r="G55" s="84"/>
+      <c r="H55" s="84"/>
+      <c r="I55" s="84"/>
+      <c r="J55" s="41"/>
+      <c r="K55" s="41"/>
+      <c r="L55" s="41"/>
+      <c r="M55" s="41"/>
+      <c r="N55" s="41"/>
+      <c r="O55" s="41"/>
+      <c r="P55" s="53"/>
+      <c r="Q55" s="54"/>
+      <c r="R55" s="41"/>
+      <c r="S55" s="41"/>
+      <c r="T55" s="41"/>
     </row>
     <row r="56" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="127" t="s">
+      <c r="A56" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="127"/>
-      <c r="C56" s="127"/>
-      <c r="D56" s="127"/>
-      <c r="E56" s="127"/>
-      <c r="F56" s="127"/>
-      <c r="G56" s="127"/>
-      <c r="H56" s="127"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="79"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="79"/>
       <c r="I56" s="5" t="s">
         <v>16</v>
       </c>
@@ -4324,25 +4066,25 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
-      <c r="P56" s="57"/>
-      <c r="Q56" s="58"/>
+      <c r="P56" s="55"/>
+      <c r="Q56" s="56"/>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
     </row>
     <row r="57" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="127"/>
-      <c r="B57" s="127"/>
-      <c r="C57" s="127"/>
-      <c r="D57" s="127"/>
-      <c r="E57" s="127"/>
-      <c r="F57" s="127"/>
-      <c r="G57" s="127"/>
-      <c r="H57" s="127"/>
+      <c r="A57" s="79"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="79"/>
+      <c r="E57" s="79"/>
+      <c r="F57" s="79"/>
+      <c r="G57" s="79"/>
+      <c r="H57" s="79"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
-      <c r="P57" s="52"/>
-      <c r="Q57" s="54"/>
+      <c r="P57" s="50"/>
+      <c r="Q57" s="52"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K58" s="2"/>
@@ -4365,7 +4107,7 @@
       <c r="N59"/>
       <c r="O59"/>
       <c r="P59"/>
-      <c r="Q59" s="49"/>
+      <c r="Q59" s="47"/>
       <c r="R59"/>
       <c r="S59"/>
       <c r="T59"/>
@@ -4392,7 +4134,7 @@
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60"/>
-      <c r="Q60" s="49"/>
+      <c r="Q60" s="47"/>
       <c r="R60"/>
       <c r="S60"/>
       <c r="T60"/>
@@ -4419,7 +4161,7 @@
       <c r="N61"/>
       <c r="O61"/>
       <c r="P61"/>
-      <c r="Q61" s="49"/>
+      <c r="Q61" s="47"/>
       <c r="R61"/>
       <c r="S61"/>
       <c r="T61"/>
@@ -4446,7 +4188,7 @@
       <c r="N62"/>
       <c r="O62"/>
       <c r="P62"/>
-      <c r="Q62" s="49"/>
+      <c r="Q62" s="47"/>
       <c r="R62"/>
       <c r="S62"/>
       <c r="T62"/>
@@ -4473,7 +4215,7 @@
       <c r="N63"/>
       <c r="O63"/>
       <c r="P63"/>
-      <c r="Q63" s="49"/>
+      <c r="Q63" s="47"/>
       <c r="R63"/>
       <c r="S63"/>
       <c r="T63"/>
@@ -4500,7 +4242,7 @@
       <c r="N64"/>
       <c r="O64"/>
       <c r="P64"/>
-      <c r="Q64" s="49"/>
+      <c r="Q64" s="47"/>
       <c r="R64"/>
       <c r="S64"/>
       <c r="T64"/>
@@ -4527,7 +4269,7 @@
       <c r="N65"/>
       <c r="O65"/>
       <c r="P65"/>
-      <c r="Q65" s="49"/>
+      <c r="Q65" s="47"/>
       <c r="R65"/>
       <c r="S65"/>
       <c r="T65"/>
@@ -4554,7 +4296,7 @@
       <c r="N66"/>
       <c r="O66"/>
       <c r="P66"/>
-      <c r="Q66" s="49"/>
+      <c r="Q66" s="47"/>
       <c r="R66"/>
       <c r="S66"/>
       <c r="T66"/>
@@ -4581,7 +4323,7 @@
       <c r="N67"/>
       <c r="O67"/>
       <c r="P67"/>
-      <c r="Q67" s="49"/>
+      <c r="Q67" s="47"/>
       <c r="R67"/>
       <c r="S67"/>
       <c r="T67"/>
@@ -4608,7 +4350,7 @@
       <c r="N68"/>
       <c r="O68"/>
       <c r="P68"/>
-      <c r="Q68" s="49"/>
+      <c r="Q68" s="47"/>
       <c r="R68"/>
       <c r="S68"/>
       <c r="T68"/>
@@ -4635,7 +4377,7 @@
       <c r="N69"/>
       <c r="O69"/>
       <c r="P69"/>
-      <c r="Q69" s="49"/>
+      <c r="Q69" s="47"/>
       <c r="R69"/>
       <c r="S69"/>
       <c r="T69"/>
@@ -4662,7 +4404,7 @@
       <c r="N70"/>
       <c r="O70"/>
       <c r="P70"/>
-      <c r="Q70" s="49"/>
+      <c r="Q70" s="47"/>
       <c r="R70"/>
       <c r="S70"/>
       <c r="T70"/>
@@ -4689,7 +4431,7 @@
       <c r="N71"/>
       <c r="O71"/>
       <c r="P71"/>
-      <c r="Q71" s="49"/>
+      <c r="Q71" s="47"/>
       <c r="R71"/>
       <c r="S71"/>
       <c r="T71"/>
@@ -4716,7 +4458,7 @@
       <c r="N72"/>
       <c r="O72"/>
       <c r="P72"/>
-      <c r="Q72" s="49"/>
+      <c r="Q72" s="47"/>
       <c r="R72"/>
       <c r="S72"/>
       <c r="T72"/>
@@ -4743,7 +4485,7 @@
       <c r="N73"/>
       <c r="O73"/>
       <c r="P73"/>
-      <c r="Q73" s="49"/>
+      <c r="Q73" s="47"/>
       <c r="R73"/>
       <c r="S73"/>
       <c r="T73"/>
@@ -4770,7 +4512,7 @@
       <c r="N74"/>
       <c r="O74"/>
       <c r="P74"/>
-      <c r="Q74" s="49"/>
+      <c r="Q74" s="47"/>
       <c r="R74"/>
       <c r="S74"/>
       <c r="T74"/>
@@ -4797,7 +4539,7 @@
       <c r="N75"/>
       <c r="O75"/>
       <c r="P75"/>
-      <c r="Q75" s="49"/>
+      <c r="Q75" s="47"/>
       <c r="R75"/>
       <c r="S75"/>
       <c r="T75"/>
@@ -4824,7 +4566,7 @@
       <c r="N76"/>
       <c r="O76"/>
       <c r="P76"/>
-      <c r="Q76" s="49"/>
+      <c r="Q76" s="47"/>
       <c r="R76"/>
       <c r="S76"/>
       <c r="T76"/>
@@ -4851,7 +4593,7 @@
       <c r="N77"/>
       <c r="O77"/>
       <c r="P77"/>
-      <c r="Q77" s="49"/>
+      <c r="Q77" s="47"/>
       <c r="R77"/>
       <c r="S77"/>
       <c r="T77"/>
@@ -4878,7 +4620,7 @@
       <c r="N78"/>
       <c r="O78"/>
       <c r="P78"/>
-      <c r="Q78" s="49"/>
+      <c r="Q78" s="47"/>
       <c r="R78"/>
       <c r="S78"/>
       <c r="T78"/>
@@ -4905,7 +4647,7 @@
       <c r="N79"/>
       <c r="O79"/>
       <c r="P79"/>
-      <c r="Q79" s="49"/>
+      <c r="Q79" s="47"/>
       <c r="R79"/>
       <c r="S79"/>
       <c r="T79"/>
@@ -4932,7 +4674,7 @@
       <c r="N80"/>
       <c r="O80"/>
       <c r="P80"/>
-      <c r="Q80" s="49"/>
+      <c r="Q80" s="47"/>
       <c r="R80"/>
       <c r="S80"/>
       <c r="T80"/>
@@ -4959,7 +4701,7 @@
       <c r="N81"/>
       <c r="O81"/>
       <c r="P81"/>
-      <c r="Q81" s="49"/>
+      <c r="Q81" s="47"/>
       <c r="R81"/>
       <c r="S81"/>
       <c r="T81"/>
@@ -4986,7 +4728,7 @@
       <c r="N82"/>
       <c r="O82"/>
       <c r="P82"/>
-      <c r="Q82" s="49"/>
+      <c r="Q82" s="47"/>
       <c r="R82"/>
       <c r="S82"/>
       <c r="T82"/>
@@ -4999,13 +4741,61 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="78">
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A56:H57"/>
-    <mergeCell ref="A53:H54"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="Y3:AA4"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E2:I3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:M5"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="J2:K3"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="K18:M18"/>
@@ -5022,61 +4812,13 @@
     <mergeCell ref="D5:E7"/>
     <mergeCell ref="F5:G7"/>
     <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="E2:I3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:M5"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="J2:K3"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="Y3:AA4"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="K46:M46"/>
-    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="A56:H57"/>
+    <mergeCell ref="A53:H54"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="A55:I55"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <dataValidations count="6">
@@ -5114,8 +4856,8 @@
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5126,303 +4868,298 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="32"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="33"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="33"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="33"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="34"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="34"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="33"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="33"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="33"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="34"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="28" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="28" t="s">
         <v>57</v>
       </c>
       <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="28" t="s">
         <v>58</v>
       </c>
       <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="28" t="s">
         <v>59</v>
       </c>
       <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="28" t="s">
         <v>70</v>
       </c>
       <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="26" t="s">
         <v>60</v>
       </c>
       <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="26" t="s">
         <v>61</v>
       </c>
       <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="26" t="s">
         <v>63</v>
       </c>
       <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="26" t="s">
         <v>64</v>
       </c>
       <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="26" t="s">
         <v>65</v>
       </c>
       <c r="G21" s="25"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="26" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="26" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="26" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="26" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="26" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="26" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="26" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="26" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="26" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="28" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="3">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
refactor: reorganize detail modal fields layout
</commit_message>
<xml_diff>
--- a/public/templates/order_template.xlsx
+++ b/public/templates/order_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\CNC_Milling\WORK_CNC\SOFT\ProjectDB\CRM\UI_ERP\React-Admin\front_Refine_v1\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACA8697-3FE6-4355-AAA9-478E20F31F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FB22AA-2DDD-4551-B832-E45E702E7EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="1845" windowWidth="16110" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="2685" windowWidth="16350" windowHeight="18210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заказ" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="МДФ">Заказ!$AK$83:$AK$87</definedName>
+    <definedName name="МДФ">Заказ!$AK$82:$AK$86</definedName>
     <definedName name="обкат">Списки!$C$2:$C$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Заказ!$A$1:$M$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Заказ!$A$1:$M$82</definedName>
     <definedName name="пленка">Списки!$E$2:$E$34</definedName>
     <definedName name="тип_детали">Списки!$A$2:$A$28</definedName>
     <definedName name="фасад">Заказ!$AI$1:$AJ$5</definedName>
@@ -649,7 +649,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -824,6 +824,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -831,7 +844,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1043,18 +1056,156 @@
     <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1064,155 +1215,23 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1522,10 +1541,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:AA82"/>
+  <dimension ref="A1:AA97"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,25 +1576,25 @@
         <v>25</v>
       </c>
       <c r="B1" s="68"/>
-      <c r="C1" s="82"/>
+      <c r="C1" s="130"/>
       <c r="D1" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="118" t="s">
+      <c r="E1" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="118"/>
-      <c r="L1" s="113" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="113"/>
+      <c r="M1" s="94"/>
       <c r="N1" s="59"/>
       <c r="P1" s="36" t="s">
         <v>87</v>
@@ -1587,25 +1606,25 @@
     <row r="2" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="80" t="s">
+      <c r="C2" s="130"/>
+      <c r="D2" s="126" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="120">
-        <f>SUM(J12:J52)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="120"/>
-      <c r="L2" s="119">
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="101">
+        <f>SUM(J12:J67)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="101"/>
+      <c r="L2" s="100">
         <f>J2-(J2*P2)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="119"/>
+      <c r="M2" s="100"/>
       <c r="N2" s="60"/>
       <c r="O2" s="37"/>
       <c r="P2" s="58"/>
@@ -1617,17 +1636,17 @@
     <row r="3" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68"/>
       <c r="B3" s="68"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
       <c r="N3" s="60"/>
       <c r="O3" s="37"/>
       <c r="P3" s="48"/>
@@ -1638,45 +1657,45 @@
       <c r="V3" s="35"/>
       <c r="W3" s="35"/>
       <c r="X3" s="35"/>
-      <c r="Y3" s="129" t="s">
+      <c r="Y3" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" s="130"/>
-      <c r="AA3" s="130"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="78"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="90" t="s">
+      <c r="B4" s="105"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="92"/>
-      <c r="F4" s="102" t="s">
+      <c r="E4" s="106"/>
+      <c r="F4" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="77" t="s">
+      <c r="G4" s="87"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="116">
+      <c r="K4" s="98">
         <f>IF(ISBLANK(L2), (J2-SUM(Q6:Q42)), (L2-SUM(Q6:Q42)))</f>
         <v>0</v>
       </c>
-      <c r="L4" s="116"/>
-      <c r="M4" s="117"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="99"/>
       <c r="N4" s="38"/>
-      <c r="O4" s="85" t="s">
+      <c r="O4" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="85" t="s">
+      <c r="P4" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="Q4" s="87" t="s">
+      <c r="Q4" s="102" t="s">
         <v>86</v>
       </c>
       <c r="R4" s="38"/>
@@ -1686,28 +1705,28 @@
       <c r="V4" s="35"/>
       <c r="W4" s="35"/>
       <c r="X4" s="35"/>
-      <c r="Y4" s="129"/>
-      <c r="Z4" s="130"/>
-      <c r="AA4" s="130"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="78"/>
     </row>
     <row r="5" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="93"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="116"/>
+      <c r="A5" s="107"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
       <c r="N5" s="38"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="87"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="102"/>
       <c r="R5" s="38"/>
       <c r="S5" s="38"/>
       <c r="T5" s="38"/>
@@ -1722,21 +1741,21 @@
       <c r="Z5" s="33"/>
     </row>
     <row r="6" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="77" t="s">
+      <c r="A6" s="108"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="89"/>
-      <c r="L6" s="89"/>
-      <c r="M6" s="89"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
       <c r="N6" s="39"/>
       <c r="O6" s="62"/>
       <c r="P6" s="63"/>
@@ -1746,19 +1765,19 @@
       <c r="T6" s="39"/>
     </row>
     <row r="7" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="94"/>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="104"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
+      <c r="A7" s="108"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
       <c r="N7" s="39"/>
       <c r="O7" s="62"/>
       <c r="P7" s="63"/>
@@ -1768,29 +1787,29 @@
       <c r="T7" s="39"/>
     </row>
     <row r="8" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="100"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="113"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="95" t="s">
+      <c r="H8" s="80"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="111">
-        <f>SUM(E12:E52)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="95" t="s">
+      <c r="K8" s="122">
+        <f>SUM(E12:E67)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="122">
-        <f>SUM(D12:D52)</f>
+      <c r="M8" s="92">
+        <f>SUM(D12:D67)</f>
         <v>0</v>
       </c>
       <c r="N8" s="14"/>
@@ -1802,19 +1821,19 @@
       <c r="T8" s="14"/>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="98"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="101"/>
+      <c r="A9" s="111"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="114"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="128"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="123"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="93"/>
       <c r="N9" s="14"/>
       <c r="O9" s="64"/>
       <c r="P9" s="8"/>
@@ -1822,7 +1841,7 @@
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
-      <c r="U9" s="118" t="s">
+      <c r="U9" s="88" t="s">
         <v>80</v>
       </c>
       <c r="V9" s="1" t="s">
@@ -1851,7 +1870,7 @@
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
-      <c r="U10" s="118"/>
+      <c r="U10" s="88"/>
     </row>
     <row r="11" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -1884,11 +1903,11 @@
       <c r="J11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="121" t="s">
+      <c r="K11" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="L11" s="121"/>
-      <c r="M11" s="121"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
       <c r="N11" s="40"/>
       <c r="O11" s="65"/>
       <c r="P11" s="66"/>
@@ -1933,9 +1952,9 @@
         <f t="shared" ref="J12:J42" si="0">E12*I12</f>
         <v>0</v>
       </c>
-      <c r="K12" s="88"/>
-      <c r="L12" s="88"/>
-      <c r="M12" s="88"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
       <c r="N12" s="5"/>
       <c r="O12" s="67"/>
       <c r="P12" s="8"/>
@@ -1987,9 +2006,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-      <c r="M13" s="88"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
       <c r="N13" s="5"/>
       <c r="O13" s="67"/>
       <c r="P13" s="8"/>
@@ -2038,9 +2057,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="88"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="76"/>
       <c r="N14" s="5"/>
       <c r="O14" s="67"/>
       <c r="P14" s="8"/>
@@ -2089,9 +2108,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="50"/>
@@ -2140,9 +2159,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="50"/>
@@ -2191,9 +2210,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K17" s="88"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="88"/>
+      <c r="K17" s="76"/>
+      <c r="L17" s="76"/>
+      <c r="M17" s="76"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="50"/>
@@ -2242,9 +2261,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="88"/>
-      <c r="L18" s="88"/>
-      <c r="M18" s="88"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="76"/>
+      <c r="M18" s="76"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="50"/>
@@ -2293,9 +2312,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K19" s="88"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="88"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="76"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="50"/>
@@ -2344,9 +2363,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="50"/>
@@ -2395,9 +2414,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="88"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="88"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="50"/>
@@ -2446,9 +2465,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="88"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="88"/>
+      <c r="K22" s="76"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="50"/>
@@ -2497,9 +2516,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="88"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="88"/>
+      <c r="K23" s="76"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="76"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="50"/>
@@ -2548,9 +2567,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="88"/>
-      <c r="L24" s="88"/>
-      <c r="M24" s="88"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="76"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="50"/>
@@ -2599,9 +2618,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="M25" s="88"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="76"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="50"/>
@@ -2650,9 +2669,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="50"/>
@@ -2701,9 +2720,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="76"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="50"/>
@@ -2752,9 +2771,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="124"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="79"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="50"/>
@@ -2803,9 +2822,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="88"/>
-      <c r="L29" s="88"/>
-      <c r="M29" s="124"/>
+      <c r="K29" s="76"/>
+      <c r="L29" s="76"/>
+      <c r="M29" s="79"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="50"/>
@@ -2854,9 +2873,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K30" s="88"/>
-      <c r="L30" s="88"/>
-      <c r="M30" s="124"/>
+      <c r="K30" s="76"/>
+      <c r="L30" s="76"/>
+      <c r="M30" s="79"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="50"/>
@@ -2905,9 +2924,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K31" s="88"/>
-      <c r="L31" s="88"/>
-      <c r="M31" s="124"/>
+      <c r="K31" s="76"/>
+      <c r="L31" s="76"/>
+      <c r="M31" s="79"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="50"/>
@@ -2956,9 +2975,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K32" s="88"/>
-      <c r="L32" s="88"/>
-      <c r="M32" s="88"/>
+      <c r="K32" s="76"/>
+      <c r="L32" s="76"/>
+      <c r="M32" s="76"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="50"/>
@@ -3007,9 +3026,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="M33" s="88"/>
+      <c r="K33" s="76"/>
+      <c r="L33" s="76"/>
+      <c r="M33" s="76"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="50"/>
@@ -3058,9 +3077,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="M34" s="88"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="50"/>
@@ -3109,9 +3128,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="88"/>
-      <c r="L35" s="88"/>
-      <c r="M35" s="88"/>
+      <c r="K35" s="76"/>
+      <c r="L35" s="76"/>
+      <c r="M35" s="76"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="50"/>
@@ -3160,9 +3179,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K36" s="88"/>
-      <c r="L36" s="88"/>
-      <c r="M36" s="88"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="50"/>
@@ -3211,9 +3230,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="88"/>
-      <c r="L37" s="88"/>
-      <c r="M37" s="88"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="50"/>
@@ -3262,9 +3281,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K38" s="88"/>
-      <c r="L38" s="88"/>
-      <c r="M38" s="88"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="76"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="50"/>
@@ -3313,9 +3332,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K39" s="88"/>
-      <c r="L39" s="88"/>
-      <c r="M39" s="88"/>
+      <c r="K39" s="76"/>
+      <c r="L39" s="76"/>
+      <c r="M39" s="76"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="50"/>
@@ -3364,9 +3383,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K40" s="88"/>
-      <c r="L40" s="88"/>
-      <c r="M40" s="88"/>
+      <c r="K40" s="76"/>
+      <c r="L40" s="76"/>
+      <c r="M40" s="76"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="50"/>
@@ -3415,9 +3434,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K41" s="88"/>
-      <c r="L41" s="88"/>
-      <c r="M41" s="88"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="76"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
       <c r="P41" s="50"/>
@@ -3466,9 +3485,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K42" s="88"/>
-      <c r="L42" s="88"/>
-      <c r="M42" s="88"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="50"/>
@@ -3506,7 +3525,7 @@
       <c r="C43" s="42"/>
       <c r="D43" s="42"/>
       <c r="E43" s="20">
-        <f t="shared" ref="E43:E51" si="8">ROUNDUP((B43/1000)*(C43/1000)*D43,2)</f>
+        <f t="shared" ref="E43:E66" si="8">ROUNDUP((B43/1000)*(C43/1000)*D43,2)</f>
         <v>0</v>
       </c>
       <c r="F43" s="20"/>
@@ -3514,12 +3533,12 @@
       <c r="H43" s="19"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9">
-        <f t="shared" ref="J43:J51" si="9">E43*I43</f>
-        <v>0</v>
-      </c>
-      <c r="K43" s="88"/>
-      <c r="L43" s="88"/>
-      <c r="M43" s="88"/>
+        <f t="shared" ref="J43:J66" si="9">E43*I43</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="76"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="50"/>
@@ -3528,24 +3547,24 @@
       <c r="S43" s="5"/>
       <c r="T43" s="19"/>
       <c r="U43" s="36">
-        <f t="shared" ref="U43:U52" si="10">IF(F43="выборка",(60),IF(F43="выборка-2ступени",(67),0))</f>
+        <f t="shared" ref="U43:U50" si="10">IF(F43="выборка",(60),IF(F43="выборка-2ступени",(67),0))</f>
         <v>0</v>
       </c>
       <c r="V43" s="36">
-        <f t="shared" ref="V43:V52" si="11">IF(AND((B43 - U43*2-1)&gt;0,U43&gt;0),B43 - U43*2-1,0)</f>
+        <f t="shared" ref="V43:V50" si="11">IF(AND((B43 - U43*2-1)&gt;0,U43&gt;0),B43 - U43*2-1,0)</f>
         <v>0</v>
       </c>
       <c r="W43" s="36">
-        <f t="shared" ref="W43:W52" si="12">IF(AND((C43 - U43*2-1)&gt;0,U43&gt;0),C43 - U43*2-1,0)</f>
+        <f t="shared" ref="W43:W50" si="12">IF(AND((C43 - U43*2-1)&gt;0,U43&gt;0),C43 - U43*2-1,0)</f>
         <v>0</v>
       </c>
       <c r="X43" s="36"/>
       <c r="Y43" s="36">
-        <f t="shared" ref="Y43:Y52" si="13">IF(F43="выборка",(B43 - 60*2-1),IF(F43="выборка-2ступени",(B43 - 67*2-1),0))</f>
+        <f t="shared" ref="Y43:Y50" si="13">IF(F43="выборка",(B43 - 60*2-1),IF(F43="выборка-2ступени",(B43 - 67*2-1),0))</f>
         <v>0</v>
       </c>
       <c r="Z43" s="36">
-        <f t="shared" ref="Z43:Z52" si="14">IF(F43="выборка",(C43 - 60*2-1),IF(F43="выборка-2ступени",(C43 - 67*2-1),0))</f>
+        <f t="shared" ref="Z43:Z50" si="14">IF(F43="выборка",(C43 - 60*2-1),IF(F43="выборка-2ступени",(C43 - 67*2-1),0))</f>
         <v>0</v>
       </c>
     </row>
@@ -3568,9 +3587,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K44" s="88"/>
-      <c r="L44" s="88"/>
-      <c r="M44" s="88"/>
+      <c r="K44" s="76"/>
+      <c r="L44" s="76"/>
+      <c r="M44" s="76"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="50"/>
@@ -3619,9 +3638,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K45" s="88"/>
-      <c r="L45" s="88"/>
-      <c r="M45" s="88"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="76"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="50"/>
@@ -3670,9 +3689,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K46" s="88"/>
-      <c r="L46" s="88"/>
-      <c r="M46" s="88"/>
+      <c r="K46" s="76"/>
+      <c r="L46" s="76"/>
+      <c r="M46" s="76"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="50"/>
@@ -3721,9 +3740,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K47" s="88"/>
-      <c r="L47" s="88"/>
-      <c r="M47" s="88"/>
+      <c r="K47" s="76"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="76"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="50"/>
@@ -3772,9 +3791,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K48" s="88"/>
-      <c r="L48" s="88"/>
-      <c r="M48" s="88"/>
+      <c r="K48" s="76"/>
+      <c r="L48" s="76"/>
+      <c r="M48" s="76"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="50"/>
@@ -3823,9 +3842,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K49" s="88"/>
-      <c r="L49" s="88"/>
-      <c r="M49" s="88"/>
+      <c r="K49" s="76"/>
+      <c r="L49" s="76"/>
+      <c r="M49" s="76"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="50"/>
@@ -3874,9 +3893,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K50" s="88"/>
-      <c r="L50" s="88"/>
-      <c r="M50" s="88"/>
+      <c r="K50" s="76"/>
+      <c r="L50" s="76"/>
+      <c r="M50" s="76"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="50"/>
@@ -3925,9 +3944,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K51" s="88"/>
-      <c r="L51" s="88"/>
-      <c r="M51" s="88"/>
+      <c r="K51" s="79"/>
+      <c r="L51" s="132"/>
+      <c r="M51" s="133"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="50"/>
@@ -3935,85 +3954,122 @@
       <c r="R51" s="5"/>
       <c r="S51" s="5"/>
       <c r="T51" s="19"/>
-      <c r="U51" s="36">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="V51" s="36">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="W51" s="36">
-        <f t="shared" si="12"/>
-        <v>0</v>
+      <c r="U51" s="36" t="e">
+        <f>IF(#REF!="выборка",(60),IF(#REF!="выборка-2ступени",(67),0))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="V51" s="36" t="e">
+        <f>IF(AND((#REF! - U51*2-1)&gt;0,U51&gt;0),#REF! - U51*2-1,0)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="W51" s="36" t="e">
+        <f>IF(AND((#REF! - U51*2-1)&gt;0,U51&gt;0),#REF! - U51*2-1,0)</f>
+        <v>#REF!</v>
       </c>
       <c r="X51" s="36"/>
-      <c r="Y51" s="36">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Z51" s="36">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y51" s="36" t="e">
+        <f>IF(#REF!="выборка",(#REF! - 60*2-1),IF(#REF!="выборка-2ступени",(#REF! - 67*2-1),0))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Z51" s="36" t="e">
+        <f>IF(#REF!="выборка",(#REF! - 60*2-1),IF(#REF!="выборка-2ступени",(#REF! - 67*2-1),0))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>41</v>
+      </c>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K52" s="79"/>
+      <c r="L52" s="132"/>
+      <c r="M52" s="133"/>
       <c r="P52" s="50"/>
       <c r="Q52" s="52"/>
       <c r="T52" s="19"/>
       <c r="U52" s="36">
-        <f t="shared" si="10"/>
+        <f>IF(F67="выборка",(60),IF(F67="выборка-2ступени",(67),0))</f>
         <v>0</v>
       </c>
       <c r="V52" s="36">
-        <f t="shared" si="11"/>
+        <f>IF(AND((B67 - U52*2-1)&gt;0,U52&gt;0),B67 - U52*2-1,0)</f>
         <v>0</v>
       </c>
       <c r="W52" s="36">
-        <f t="shared" si="12"/>
+        <f>IF(AND((C67 - U52*2-1)&gt;0,U52&gt;0),C67 - U52*2-1,0)</f>
         <v>0</v>
       </c>
       <c r="X52" s="36"/>
       <c r="Y52" s="36">
-        <f t="shared" si="13"/>
+        <f>IF(F67="выборка",(B67 - 60*2-1),IF(F67="выборка-2ступени",(B67 - 67*2-1),0))</f>
         <v>0</v>
       </c>
       <c r="Z52" s="36">
-        <f t="shared" si="14"/>
+        <f>IF(F67="выборка",(C67 - 60*2-1),IF(F67="выборка-2ступени",(C67 - 67*2-1),0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:26" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="79" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="79"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A53" s="8">
+        <v>42</v>
+      </c>
+      <c r="B53" s="42"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K53" s="79"/>
+      <c r="L53" s="132"/>
+      <c r="M53" s="133"/>
       <c r="P53" s="50"/>
       <c r="Q53" s="52"/>
     </row>
     <row r="54" spans="1:26" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="79"/>
-      <c r="B54" s="79"/>
-      <c r="C54" s="79"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="79"/>
-      <c r="G54" s="79"/>
-      <c r="H54" s="79"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
+      <c r="A54" s="8">
+        <v>43</v>
+      </c>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="79"/>
+      <c r="L54" s="132"/>
+      <c r="M54" s="133"/>
       <c r="N54" s="41"/>
       <c r="O54" s="41"/>
       <c r="P54" s="53"/>
@@ -4023,21 +4079,27 @@
       <c r="T54" s="41"/>
     </row>
     <row r="55" spans="1:26" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="84" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55" s="84"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="84"/>
-      <c r="F55" s="84"/>
-      <c r="G55" s="84"/>
-      <c r="H55" s="84"/>
-      <c r="I55" s="84"/>
-      <c r="J55" s="41"/>
-      <c r="K55" s="41"/>
-      <c r="L55" s="41"/>
-      <c r="M55" s="41"/>
+      <c r="A55" s="8">
+        <v>44</v>
+      </c>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K55" s="79"/>
+      <c r="L55" s="132"/>
+      <c r="M55" s="133"/>
       <c r="N55" s="41"/>
       <c r="O55" s="41"/>
       <c r="P55" s="53"/>
@@ -4047,23 +4109,27 @@
       <c r="T55" s="41"/>
     </row>
     <row r="56" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="79" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="79"/>
-      <c r="C56" s="79"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="79"/>
-      <c r="F56" s="79"/>
-      <c r="G56" s="79"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
+      <c r="A56" s="8">
+        <v>45</v>
+      </c>
+      <c r="B56" s="42"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K56" s="79"/>
+      <c r="L56" s="132"/>
+      <c r="M56" s="133"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" s="55"/>
@@ -4073,37 +4139,75 @@
       <c r="T56" s="2"/>
     </row>
     <row r="57" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="79"/>
-      <c r="B57" s="79"/>
-      <c r="C57" s="79"/>
-      <c r="D57" s="79"/>
-      <c r="E57" s="79"/>
-      <c r="F57" s="79"/>
-      <c r="G57" s="79"/>
-      <c r="H57" s="79"/>
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
+      <c r="A57" s="8">
+        <v>46</v>
+      </c>
+      <c r="B57" s="42"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K57" s="79"/>
+      <c r="L57" s="132"/>
+      <c r="M57" s="133"/>
       <c r="P57" s="50"/>
       <c r="Q57" s="52"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="D59"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
-      <c r="J59"/>
-      <c r="K59"/>
-      <c r="L59"/>
-      <c r="M59"/>
+    <row r="58" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>47</v>
+      </c>
+      <c r="B58" s="42"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K58" s="79"/>
+      <c r="L58" s="132"/>
+      <c r="M58" s="133"/>
+    </row>
+    <row r="59" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
+        <v>48</v>
+      </c>
+      <c r="B59" s="42"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K59" s="79"/>
+      <c r="L59" s="132"/>
+      <c r="M59" s="133"/>
       <c r="N59"/>
       <c r="O59"/>
       <c r="P59"/>
@@ -4117,20 +4221,28 @@
       <c r="X59"/>
       <c r="Y59"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
-      <c r="J60"/>
-      <c r="K60"/>
-      <c r="L60"/>
-      <c r="M60"/>
+    <row r="60" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>49</v>
+      </c>
+      <c r="B60" s="42"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K60" s="79"/>
+      <c r="L60" s="132"/>
+      <c r="M60" s="133"/>
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60"/>
@@ -4144,20 +4256,28 @@
       <c r="X60"/>
       <c r="Y60"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-      <c r="J61"/>
-      <c r="K61"/>
-      <c r="L61"/>
-      <c r="M61"/>
+    <row r="61" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
+        <v>50</v>
+      </c>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K61" s="79"/>
+      <c r="L61" s="132"/>
+      <c r="M61" s="133"/>
       <c r="N61"/>
       <c r="O61"/>
       <c r="P61"/>
@@ -4171,20 +4291,28 @@
       <c r="X61"/>
       <c r="Y61"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
-      <c r="J62"/>
-      <c r="K62"/>
-      <c r="L62"/>
-      <c r="M62"/>
+    <row r="62" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
+        <v>51</v>
+      </c>
+      <c r="B62" s="42"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K62" s="79"/>
+      <c r="L62" s="132"/>
+      <c r="M62" s="133"/>
       <c r="N62"/>
       <c r="O62"/>
       <c r="P62"/>
@@ -4198,20 +4326,28 @@
       <c r="X62"/>
       <c r="Y62"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
-      <c r="J63"/>
-      <c r="K63"/>
-      <c r="L63"/>
-      <c r="M63"/>
+    <row r="63" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8">
+        <v>52</v>
+      </c>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K63" s="79"/>
+      <c r="L63" s="132"/>
+      <c r="M63" s="133"/>
       <c r="N63"/>
       <c r="O63"/>
       <c r="P63"/>
@@ -4225,20 +4361,28 @@
       <c r="X63"/>
       <c r="Y63"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
-      <c r="J64"/>
-      <c r="K64"/>
-      <c r="L64"/>
-      <c r="M64"/>
+    <row r="64" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8">
+        <v>53</v>
+      </c>
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K64" s="79"/>
+      <c r="L64" s="132"/>
+      <c r="M64" s="133"/>
       <c r="N64"/>
       <c r="O64"/>
       <c r="P64"/>
@@ -4252,20 +4396,28 @@
       <c r="X64"/>
       <c r="Y64"/>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
-      <c r="J65"/>
-      <c r="K65"/>
-      <c r="L65"/>
-      <c r="M65"/>
+    <row r="65" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8">
+        <v>54</v>
+      </c>
+      <c r="B65" s="42"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K65" s="79"/>
+      <c r="L65" s="132"/>
+      <c r="M65" s="133"/>
       <c r="N65"/>
       <c r="O65"/>
       <c r="P65"/>
@@ -4279,20 +4431,28 @@
       <c r="X65"/>
       <c r="Y65"/>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
-      <c r="J66"/>
-      <c r="K66"/>
-      <c r="L66"/>
-      <c r="M66"/>
+    <row r="66" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
+        <v>55</v>
+      </c>
+      <c r="B66" s="42"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K66" s="79"/>
+      <c r="L66" s="132"/>
+      <c r="M66" s="133"/>
       <c r="N66"/>
       <c r="O66"/>
       <c r="P66"/>
@@ -4307,19 +4467,6 @@
       <c r="Y66"/>
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="D67"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
-      <c r="J67"/>
-      <c r="K67"/>
-      <c r="L67"/>
-      <c r="M67"/>
       <c r="N67"/>
       <c r="O67"/>
       <c r="P67"/>
@@ -4334,19 +4481,19 @@
       <c r="Y67"/>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="D68"/>
-      <c r="E68"/>
-      <c r="F68"/>
-      <c r="G68"/>
-      <c r="H68"/>
-      <c r="I68"/>
-      <c r="J68"/>
-      <c r="K68"/>
-      <c r="L68"/>
-      <c r="M68"/>
+      <c r="A68" s="125" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="125"/>
+      <c r="C68" s="125"/>
+      <c r="D68" s="125"/>
+      <c r="E68" s="125"/>
+      <c r="F68" s="125"/>
+      <c r="G68" s="125"/>
+      <c r="H68" s="125"/>
+      <c r="I68" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="N68"/>
       <c r="O68"/>
       <c r="P68"/>
@@ -4361,19 +4508,19 @@
       <c r="Y68"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="D69"/>
-      <c r="E69"/>
-      <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
-      <c r="J69"/>
-      <c r="K69"/>
-      <c r="L69"/>
-      <c r="M69"/>
+      <c r="A69" s="125"/>
+      <c r="B69" s="125"/>
+      <c r="C69" s="125"/>
+      <c r="D69" s="125"/>
+      <c r="E69" s="125"/>
+      <c r="F69" s="125"/>
+      <c r="G69" s="125"/>
+      <c r="H69" s="125"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
       <c r="N69"/>
       <c r="O69"/>
       <c r="P69"/>
@@ -4388,19 +4535,21 @@
       <c r="Y69"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
-      <c r="F70"/>
-      <c r="G70"/>
-      <c r="H70"/>
-      <c r="I70"/>
-      <c r="J70"/>
-      <c r="K70"/>
-      <c r="L70"/>
-      <c r="M70"/>
+      <c r="A70" s="128" t="s">
+        <v>103</v>
+      </c>
+      <c r="B70" s="128"/>
+      <c r="C70" s="128"/>
+      <c r="D70" s="128"/>
+      <c r="E70" s="128"/>
+      <c r="F70" s="128"/>
+      <c r="G70" s="128"/>
+      <c r="H70" s="128"/>
+      <c r="I70" s="128"/>
+      <c r="J70" s="41"/>
+      <c r="K70" s="41"/>
+      <c r="L70" s="41"/>
+      <c r="M70" s="41"/>
       <c r="N70"/>
       <c r="O70"/>
       <c r="P70"/>
@@ -4415,19 +4564,23 @@
       <c r="Y70"/>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
-      <c r="J71"/>
-      <c r="K71"/>
-      <c r="L71"/>
-      <c r="M71"/>
+      <c r="A71" s="125" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="125"/>
+      <c r="C71" s="125"/>
+      <c r="D71" s="125"/>
+      <c r="E71" s="125"/>
+      <c r="F71" s="125"/>
+      <c r="G71" s="125"/>
+      <c r="H71" s="125"/>
+      <c r="I71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
       <c r="N71"/>
       <c r="O71"/>
       <c r="P71"/>
@@ -4442,19 +4595,16 @@
       <c r="Y71"/>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A72"/>
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="D72"/>
-      <c r="E72"/>
-      <c r="F72"/>
-      <c r="G72"/>
-      <c r="H72"/>
-      <c r="I72"/>
-      <c r="J72"/>
-      <c r="K72"/>
-      <c r="L72"/>
-      <c r="M72"/>
+      <c r="A72" s="125"/>
+      <c r="B72" s="125"/>
+      <c r="C72" s="125"/>
+      <c r="D72" s="125"/>
+      <c r="E72" s="125"/>
+      <c r="F72" s="125"/>
+      <c r="G72" s="125"/>
+      <c r="H72" s="125"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
       <c r="N72"/>
       <c r="O72"/>
       <c r="P72"/>
@@ -4469,19 +4619,8 @@
       <c r="Y72"/>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A73"/>
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="D73"/>
-      <c r="E73"/>
-      <c r="F73"/>
-      <c r="G73"/>
-      <c r="H73"/>
-      <c r="I73"/>
-      <c r="J73"/>
-      <c r="K73"/>
-      <c r="L73"/>
-      <c r="M73"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
       <c r="N73"/>
       <c r="O73"/>
       <c r="P73"/>
@@ -4725,31 +4864,297 @@
       <c r="K82"/>
       <c r="L82"/>
       <c r="M82"/>
-      <c r="N82"/>
-      <c r="O82"/>
-      <c r="P82"/>
-      <c r="Q82" s="47"/>
-      <c r="R82"/>
-      <c r="S82"/>
-      <c r="T82"/>
-      <c r="U82"/>
-      <c r="V82"/>
-      <c r="W82"/>
-      <c r="X82"/>
-      <c r="Y82"/>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83"/>
+      <c r="J83"/>
+      <c r="K83"/>
+      <c r="L83"/>
+      <c r="M83"/>
+    </row>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84"/>
+      <c r="J84"/>
+      <c r="K84"/>
+      <c r="L84"/>
+      <c r="M84"/>
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
+      <c r="J85"/>
+      <c r="K85"/>
+      <c r="L85"/>
+      <c r="M85"/>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
+      <c r="J86"/>
+      <c r="K86"/>
+      <c r="L86"/>
+      <c r="M86"/>
+    </row>
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="I87"/>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="L87"/>
+      <c r="M87"/>
+    </row>
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A88"/>
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+      <c r="J88"/>
+      <c r="K88"/>
+      <c r="L88"/>
+      <c r="M88"/>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
+      <c r="M89"/>
+    </row>
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90"/>
+      <c r="M90"/>
+    </row>
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A91"/>
+      <c r="B91"/>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+      <c r="M91"/>
+    </row>
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A92"/>
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92"/>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="L92"/>
+      <c r="M92"/>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+    </row>
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95"/>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96"/>
+      <c r="M96"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97"/>
+      <c r="B97"/>
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="E97"/>
+      <c r="F97"/>
+      <c r="G97"/>
+      <c r="H97"/>
+      <c r="I97"/>
+      <c r="J97"/>
+      <c r="K97"/>
+      <c r="L97"/>
+      <c r="M97"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="78">
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="K46:M46"/>
-    <mergeCell ref="K47:M47"/>
+  <mergeCells count="93">
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="K63:M63"/>
+    <mergeCell ref="K64:M64"/>
+    <mergeCell ref="K65:M65"/>
+    <mergeCell ref="K57:M57"/>
+    <mergeCell ref="K58:M58"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="A71:H72"/>
+    <mergeCell ref="A68:H69"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="A70:I70"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K6:M7"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="D5:E7"/>
+    <mergeCell ref="F5:G7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E2:I3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:M5"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="J2:K3"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K17:M17"/>
     <mergeCell ref="Y3:AA4"/>
     <mergeCell ref="K41:M41"/>
     <mergeCell ref="K42:M42"/>
@@ -4766,78 +5171,40 @@
     <mergeCell ref="K38:M38"/>
     <mergeCell ref="K27:M27"/>
     <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="E2:I3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:M5"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="J2:K3"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K6:M7"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="D5:E7"/>
-    <mergeCell ref="F5:G7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A56:H57"/>
-    <mergeCell ref="A53:H54"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="K66:M66"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="K55:M55"/>
+    <mergeCell ref="K56:M56"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" sqref="A5:C7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>тип_детали</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:E7 G12:G51" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:E7 G12:G66" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>обкат</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:G7" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>пленка</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I12:I51" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I12:I66" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>цена_кв_м</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F12:F51" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F12:F66" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>тип_детали</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H12:H51" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" sqref="H12:H66" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>пленка</formula1>
     </dataValidation>
   </dataValidations>
@@ -4871,10 +5238,10 @@
       <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="131" t="s">
+      <c r="C1" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="131" t="s">
+      <c r="E1" s="75" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="29"/>

</xml_diff>

<commit_message>
feat(orders): add client phone to Excel and GDrive export
</commit_message>
<xml_diff>
--- a/public/templates/order_template.xlsx
+++ b/public/templates/order_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\CNC_Milling\WORK_CNC\SOFT\ProjectDB\CRM\UI_ERP\React-Admin\front_Refine_v1\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FB22AA-2DDD-4551-B832-E45E702E7EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CFD1E0-8F68-44DC-B68C-9D59274D47B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="2685" windowWidth="16350" windowHeight="18210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="3390" windowWidth="16350" windowHeight="18210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заказ" sheetId="1" r:id="rId1"/>
@@ -463,13 +463,6 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Bodoni MT"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -627,6 +620,14 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -891,10 +892,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -912,7 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -961,14 +962,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -978,28 +979,28 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1008,21 +1009,24 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1032,9 +1036,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1047,18 +1048,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1068,25 +1078,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1113,13 +1108,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,13 +1126,13 @@
     <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1176,6 +1171,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1209,29 +1207,32 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1544,7 +1545,7 @@
   <dimension ref="A1:AA97"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+      <selection activeCell="H8" sqref="H8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,25 +1577,25 @@
         <v>25</v>
       </c>
       <c r="B1" s="68"/>
-      <c r="C1" s="130"/>
+      <c r="C1" s="127"/>
       <c r="D1" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="88" t="s">
+      <c r="E1" s="93" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="94" t="s">
+      <c r="K1" s="86"/>
+      <c r="L1" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="94"/>
+      <c r="M1" s="92"/>
       <c r="N1" s="59"/>
       <c r="P1" s="36" t="s">
         <v>87</v>
@@ -1606,25 +1607,25 @@
     <row r="2" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="126" t="s">
+      <c r="C2" s="127"/>
+      <c r="D2" s="125" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="101">
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="99">
         <f>SUM(J12:J67)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="101"/>
-      <c r="L2" s="100">
+      <c r="K2" s="99"/>
+      <c r="L2" s="98">
         <f>J2-(J2*P2)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="100"/>
+      <c r="M2" s="98"/>
       <c r="N2" s="60"/>
       <c r="O2" s="37"/>
       <c r="P2" s="58"/>
@@ -1636,17 +1637,17 @@
     <row r="3" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68"/>
       <c r="B3" s="68"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
       <c r="N3" s="60"/>
       <c r="O3" s="37"/>
       <c r="P3" s="48"/>
@@ -1657,45 +1658,45 @@
       <c r="V3" s="35"/>
       <c r="W3" s="35"/>
       <c r="X3" s="35"/>
-      <c r="Y3" s="77" t="s">
+      <c r="Y3" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
+      <c r="Z3" s="81"/>
+      <c r="AA3" s="81"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="105"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="104" t="s">
+      <c r="B4" s="103"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="106"/>
-      <c r="F4" s="86" t="s">
+      <c r="E4" s="104"/>
+      <c r="F4" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="97" t="s">
+      <c r="G4" s="85"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="98">
+      <c r="K4" s="96">
         <f>IF(ISBLANK(L2), (J2-SUM(Q6:Q42)), (L2-SUM(Q6:Q42)))</f>
         <v>0</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="99"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="97"/>
       <c r="N4" s="38"/>
-      <c r="O4" s="84" t="s">
+      <c r="O4" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="Q4" s="102" t="s">
+      <c r="Q4" s="100" t="s">
         <v>86</v>
       </c>
       <c r="R4" s="38"/>
@@ -1705,28 +1706,28 @@
       <c r="V4" s="35"/>
       <c r="W4" s="35"/>
       <c r="X4" s="35"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="81"/>
+      <c r="AA4" s="81"/>
     </row>
     <row r="5" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="117"/>
-      <c r="H5" s="129"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="96"/>
       <c r="N5" s="38"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="102"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="100"/>
       <c r="R5" s="38"/>
       <c r="S5" s="38"/>
       <c r="T5" s="38"/>
@@ -1741,21 +1742,21 @@
       <c r="Z5" s="33"/>
     </row>
     <row r="6" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
-      <c r="B6" s="108"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="97" t="s">
+      <c r="A6" s="106"/>
+      <c r="B6" s="106"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="101"/>
       <c r="N6" s="39"/>
       <c r="O6" s="62"/>
       <c r="P6" s="63"/>
@@ -1765,19 +1766,19 @@
       <c r="T6" s="39"/>
     </row>
     <row r="7" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="108"/>
-      <c r="B7" s="108"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
+      <c r="A7" s="106"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
       <c r="N7" s="39"/>
       <c r="O7" s="62"/>
       <c r="P7" s="63"/>
@@ -1787,28 +1788,28 @@
       <c r="T7" s="39"/>
     </row>
     <row r="8" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="109" t="s">
+      <c r="A8" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="110"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="113"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="111"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="90" t="s">
+      <c r="H8" s="133"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="122">
+      <c r="K8" s="121">
         <f>SUM(E12:E67)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="90" t="s">
+      <c r="L8" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="92">
+      <c r="M8" s="90">
         <f>SUM(D12:D67)</f>
         <v>0</v>
       </c>
@@ -1821,19 +1822,19 @@
       <c r="T8" s="14"/>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="111"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="115"/>
-      <c r="D9" s="115"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="114"/>
+      <c r="A9" s="109"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="112"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="91"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="91"/>
-      <c r="M9" s="93"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="91"/>
       <c r="N9" s="14"/>
       <c r="O9" s="64"/>
       <c r="P9" s="8"/>
@@ -1841,7 +1842,7 @@
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
-      <c r="U9" s="88" t="s">
+      <c r="U9" s="86" t="s">
         <v>80</v>
       </c>
       <c r="V9" s="1" t="s">
@@ -1870,7 +1871,7 @@
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
-      <c r="U10" s="88"/>
+      <c r="U10" s="86"/>
     </row>
     <row r="11" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -1903,11 +1904,11 @@
       <c r="J11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="89" t="s">
+      <c r="K11" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="L11" s="89"/>
-      <c r="M11" s="89"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
       <c r="N11" s="40"/>
       <c r="O11" s="65"/>
       <c r="P11" s="66"/>
@@ -1952,9 +1953,9 @@
         <f t="shared" ref="J12:J42" si="0">E12*I12</f>
         <v>0</v>
       </c>
-      <c r="K12" s="76"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="76"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
       <c r="N12" s="5"/>
       <c r="O12" s="67"/>
       <c r="P12" s="8"/>
@@ -2006,9 +2007,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="76"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
       <c r="N13" s="5"/>
       <c r="O13" s="67"/>
       <c r="P13" s="8"/>
@@ -2057,9 +2058,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="76"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
       <c r="N14" s="5"/>
       <c r="O14" s="67"/>
       <c r="P14" s="8"/>
@@ -2108,9 +2109,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="50"/>
@@ -2159,9 +2160,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="50"/>
@@ -2210,9 +2211,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="50"/>
@@ -2261,9 +2262,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="50"/>
@@ -2312,9 +2313,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="76"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="50"/>
@@ -2363,9 +2364,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="76"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="79"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="50"/>
@@ -2414,9 +2415,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="76"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="76"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="50"/>
@@ -2465,9 +2466,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="76"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="76"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="79"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="50"/>
@@ -2516,9 +2517,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="76"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="76"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="50"/>
@@ -2567,9 +2568,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="76"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="76"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="50"/>
@@ -2618,9 +2619,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="76"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="76"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="50"/>
@@ -2669,9 +2670,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="76"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="79"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="50"/>
@@ -2720,9 +2721,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="76"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="50"/>
@@ -2771,9 +2772,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K28" s="76"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="79"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="79"/>
+      <c r="M28" s="76"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="50"/>
@@ -2822,9 +2823,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="76"/>
-      <c r="L29" s="76"/>
-      <c r="M29" s="79"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="79"/>
+      <c r="M29" s="76"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="50"/>
@@ -2873,9 +2874,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K30" s="76"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="76"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="50"/>
@@ -2924,9 +2925,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K31" s="76"/>
-      <c r="L31" s="76"/>
-      <c r="M31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="76"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="50"/>
@@ -2975,9 +2976,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K32" s="76"/>
-      <c r="L32" s="76"/>
-      <c r="M32" s="76"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="79"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="50"/>
@@ -3026,9 +3027,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K33" s="76"/>
-      <c r="L33" s="76"/>
-      <c r="M33" s="76"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="79"/>
+      <c r="M33" s="79"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="50"/>
@@ -3077,9 +3078,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K34" s="76"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="76"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="79"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="50"/>
@@ -3128,9 +3129,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="76"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="76"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="50"/>
@@ -3179,9 +3180,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="79"/>
+      <c r="M36" s="79"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="50"/>
@@ -3230,9 +3231,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="76"/>
-      <c r="L37" s="76"/>
-      <c r="M37" s="76"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="79"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="50"/>
@@ -3281,9 +3282,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K38" s="76"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="76"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="50"/>
@@ -3332,9 +3333,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K39" s="76"/>
-      <c r="L39" s="76"/>
-      <c r="M39" s="76"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="50"/>
@@ -3383,9 +3384,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K40" s="76"/>
-      <c r="L40" s="76"/>
-      <c r="M40" s="76"/>
+      <c r="K40" s="79"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="79"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="50"/>
@@ -3434,9 +3435,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K41" s="76"/>
-      <c r="L41" s="76"/>
-      <c r="M41" s="76"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="79"/>
+      <c r="M41" s="79"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
       <c r="P41" s="50"/>
@@ -3485,9 +3486,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K42" s="76"/>
-      <c r="L42" s="76"/>
-      <c r="M42" s="76"/>
+      <c r="K42" s="79"/>
+      <c r="L42" s="79"/>
+      <c r="M42" s="79"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="50"/>
@@ -3536,9 +3537,9 @@
         <f t="shared" ref="J43:J66" si="9">E43*I43</f>
         <v>0</v>
       </c>
-      <c r="K43" s="76"/>
-      <c r="L43" s="76"/>
-      <c r="M43" s="76"/>
+      <c r="K43" s="79"/>
+      <c r="L43" s="79"/>
+      <c r="M43" s="79"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="50"/>
@@ -3587,9 +3588,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K44" s="76"/>
-      <c r="L44" s="76"/>
-      <c r="M44" s="76"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="79"/>
+      <c r="M44" s="79"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="50"/>
@@ -3638,9 +3639,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K45" s="76"/>
-      <c r="L45" s="76"/>
-      <c r="M45" s="76"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="79"/>
+      <c r="M45" s="79"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="50"/>
@@ -3689,9 +3690,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K46" s="76"/>
-      <c r="L46" s="76"/>
-      <c r="M46" s="76"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="79"/>
+      <c r="M46" s="79"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="50"/>
@@ -3740,9 +3741,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K47" s="76"/>
-      <c r="L47" s="76"/>
-      <c r="M47" s="76"/>
+      <c r="K47" s="79"/>
+      <c r="L47" s="79"/>
+      <c r="M47" s="79"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="50"/>
@@ -3791,9 +3792,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K48" s="76"/>
-      <c r="L48" s="76"/>
-      <c r="M48" s="76"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="79"/>
+      <c r="M48" s="79"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="50"/>
@@ -3842,9 +3843,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K49" s="76"/>
-      <c r="L49" s="76"/>
-      <c r="M49" s="76"/>
+      <c r="K49" s="79"/>
+      <c r="L49" s="79"/>
+      <c r="M49" s="79"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="50"/>
@@ -3893,9 +3894,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K50" s="76"/>
-      <c r="L50" s="76"/>
-      <c r="M50" s="76"/>
+      <c r="K50" s="79"/>
+      <c r="L50" s="79"/>
+      <c r="M50" s="79"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="50"/>
@@ -3944,9 +3945,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K51" s="79"/>
-      <c r="L51" s="132"/>
-      <c r="M51" s="133"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="77"/>
+      <c r="M51" s="78"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="50"/>
@@ -3995,9 +3996,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K52" s="79"/>
-      <c r="L52" s="132"/>
-      <c r="M52" s="133"/>
+      <c r="K52" s="76"/>
+      <c r="L52" s="77"/>
+      <c r="M52" s="78"/>
       <c r="P52" s="50"/>
       <c r="Q52" s="52"/>
       <c r="T52" s="19"/>
@@ -4042,9 +4043,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K53" s="79"/>
-      <c r="L53" s="132"/>
-      <c r="M53" s="133"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="77"/>
+      <c r="M53" s="78"/>
       <c r="P53" s="50"/>
       <c r="Q53" s="52"/>
     </row>
@@ -4067,9 +4068,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K54" s="79"/>
-      <c r="L54" s="132"/>
-      <c r="M54" s="133"/>
+      <c r="K54" s="76"/>
+      <c r="L54" s="77"/>
+      <c r="M54" s="78"/>
       <c r="N54" s="41"/>
       <c r="O54" s="41"/>
       <c r="P54" s="53"/>
@@ -4097,9 +4098,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K55" s="79"/>
-      <c r="L55" s="132"/>
-      <c r="M55" s="133"/>
+      <c r="K55" s="76"/>
+      <c r="L55" s="77"/>
+      <c r="M55" s="78"/>
       <c r="N55" s="41"/>
       <c r="O55" s="41"/>
       <c r="P55" s="53"/>
@@ -4127,9 +4128,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K56" s="79"/>
-      <c r="L56" s="132"/>
-      <c r="M56" s="133"/>
+      <c r="K56" s="76"/>
+      <c r="L56" s="77"/>
+      <c r="M56" s="78"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" s="55"/>
@@ -4157,9 +4158,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K57" s="79"/>
-      <c r="L57" s="132"/>
-      <c r="M57" s="133"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="77"/>
+      <c r="M57" s="78"/>
       <c r="P57" s="50"/>
       <c r="Q57" s="52"/>
     </row>
@@ -4182,9 +4183,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K58" s="79"/>
-      <c r="L58" s="132"/>
-      <c r="M58" s="133"/>
+      <c r="K58" s="76"/>
+      <c r="L58" s="77"/>
+      <c r="M58" s="78"/>
     </row>
     <row r="59" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
@@ -4205,9 +4206,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K59" s="79"/>
-      <c r="L59" s="132"/>
-      <c r="M59" s="133"/>
+      <c r="K59" s="76"/>
+      <c r="L59" s="77"/>
+      <c r="M59" s="78"/>
       <c r="N59"/>
       <c r="O59"/>
       <c r="P59"/>
@@ -4240,9 +4241,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K60" s="79"/>
-      <c r="L60" s="132"/>
-      <c r="M60" s="133"/>
+      <c r="K60" s="76"/>
+      <c r="L60" s="77"/>
+      <c r="M60" s="78"/>
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60"/>
@@ -4275,9 +4276,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K61" s="79"/>
-      <c r="L61" s="132"/>
-      <c r="M61" s="133"/>
+      <c r="K61" s="76"/>
+      <c r="L61" s="77"/>
+      <c r="M61" s="78"/>
       <c r="N61"/>
       <c r="O61"/>
       <c r="P61"/>
@@ -4310,9 +4311,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K62" s="79"/>
-      <c r="L62" s="132"/>
-      <c r="M62" s="133"/>
+      <c r="K62" s="76"/>
+      <c r="L62" s="77"/>
+      <c r="M62" s="78"/>
       <c r="N62"/>
       <c r="O62"/>
       <c r="P62"/>
@@ -4345,9 +4346,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K63" s="79"/>
-      <c r="L63" s="132"/>
-      <c r="M63" s="133"/>
+      <c r="K63" s="76"/>
+      <c r="L63" s="77"/>
+      <c r="M63" s="78"/>
       <c r="N63"/>
       <c r="O63"/>
       <c r="P63"/>
@@ -4380,9 +4381,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K64" s="79"/>
-      <c r="L64" s="132"/>
-      <c r="M64" s="133"/>
+      <c r="K64" s="76"/>
+      <c r="L64" s="77"/>
+      <c r="M64" s="78"/>
       <c r="N64"/>
       <c r="O64"/>
       <c r="P64"/>
@@ -4415,9 +4416,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K65" s="79"/>
-      <c r="L65" s="132"/>
-      <c r="M65" s="133"/>
+      <c r="K65" s="76"/>
+      <c r="L65" s="77"/>
+      <c r="M65" s="78"/>
       <c r="N65"/>
       <c r="O65"/>
       <c r="P65"/>
@@ -4450,9 +4451,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K66" s="79"/>
-      <c r="L66" s="132"/>
-      <c r="M66" s="133"/>
+      <c r="K66" s="76"/>
+      <c r="L66" s="77"/>
+      <c r="M66" s="78"/>
       <c r="N66"/>
       <c r="O66"/>
       <c r="P66"/>
@@ -4481,16 +4482,16 @@
       <c r="Y67"/>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A68" s="125" t="s">
+      <c r="A68" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="B68" s="125"/>
-      <c r="C68" s="125"/>
-      <c r="D68" s="125"/>
-      <c r="E68" s="125"/>
-      <c r="F68" s="125"/>
-      <c r="G68" s="125"/>
-      <c r="H68" s="125"/>
+      <c r="B68" s="124"/>
+      <c r="C68" s="124"/>
+      <c r="D68" s="124"/>
+      <c r="E68" s="124"/>
+      <c r="F68" s="124"/>
+      <c r="G68" s="124"/>
+      <c r="H68" s="124"/>
       <c r="I68" s="4" t="s">
         <v>15</v>
       </c>
@@ -4508,14 +4509,14 @@
       <c r="Y68"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A69" s="125"/>
-      <c r="B69" s="125"/>
-      <c r="C69" s="125"/>
-      <c r="D69" s="125"/>
-      <c r="E69" s="125"/>
-      <c r="F69" s="125"/>
-      <c r="G69" s="125"/>
-      <c r="H69" s="125"/>
+      <c r="A69" s="124"/>
+      <c r="B69" s="124"/>
+      <c r="C69" s="124"/>
+      <c r="D69" s="124"/>
+      <c r="E69" s="124"/>
+      <c r="F69" s="124"/>
+      <c r="G69" s="124"/>
+      <c r="H69" s="124"/>
       <c r="I69" s="3"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
@@ -4535,17 +4536,17 @@
       <c r="Y69"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A70" s="128" t="s">
+      <c r="A70" s="129" t="s">
         <v>103</v>
       </c>
-      <c r="B70" s="128"/>
-      <c r="C70" s="128"/>
-      <c r="D70" s="128"/>
-      <c r="E70" s="128"/>
-      <c r="F70" s="128"/>
-      <c r="G70" s="128"/>
-      <c r="H70" s="128"/>
-      <c r="I70" s="128"/>
+      <c r="B70" s="129"/>
+      <c r="C70" s="129"/>
+      <c r="D70" s="129"/>
+      <c r="E70" s="129"/>
+      <c r="F70" s="129"/>
+      <c r="G70" s="129"/>
+      <c r="H70" s="129"/>
+      <c r="I70" s="129"/>
       <c r="J70" s="41"/>
       <c r="K70" s="41"/>
       <c r="L70" s="41"/>
@@ -4564,16 +4565,16 @@
       <c r="Y70"/>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A71" s="125" t="s">
+      <c r="A71" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="B71" s="125"/>
-      <c r="C71" s="125"/>
-      <c r="D71" s="125"/>
-      <c r="E71" s="125"/>
-      <c r="F71" s="125"/>
-      <c r="G71" s="125"/>
-      <c r="H71" s="125"/>
+      <c r="B71" s="124"/>
+      <c r="C71" s="124"/>
+      <c r="D71" s="124"/>
+      <c r="E71" s="124"/>
+      <c r="F71" s="124"/>
+      <c r="G71" s="124"/>
+      <c r="H71" s="124"/>
       <c r="I71" s="5" t="s">
         <v>16</v>
       </c>
@@ -4595,14 +4596,14 @@
       <c r="Y71"/>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A72" s="125"/>
-      <c r="B72" s="125"/>
-      <c r="C72" s="125"/>
-      <c r="D72" s="125"/>
-      <c r="E72" s="125"/>
-      <c r="F72" s="125"/>
-      <c r="G72" s="125"/>
-      <c r="H72" s="125"/>
+      <c r="A72" s="124"/>
+      <c r="B72" s="124"/>
+      <c r="C72" s="124"/>
+      <c r="D72" s="124"/>
+      <c r="E72" s="124"/>
+      <c r="F72" s="124"/>
+      <c r="G72" s="124"/>
+      <c r="H72" s="124"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="N72"/>
@@ -5093,15 +5094,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="93">
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="K63:M63"/>
-    <mergeCell ref="K64:M64"/>
-    <mergeCell ref="K65:M65"/>
-    <mergeCell ref="K57:M57"/>
-    <mergeCell ref="K58:M58"/>
-    <mergeCell ref="K59:M59"/>
-    <mergeCell ref="K60:M60"/>
-    <mergeCell ref="K61:M61"/>
     <mergeCell ref="C8:E9"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="A71:H72"/>
@@ -5186,8 +5178,17 @@
     <mergeCell ref="K54:M54"/>
     <mergeCell ref="K55:M55"/>
     <mergeCell ref="K56:M56"/>
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="K63:M63"/>
+    <mergeCell ref="K64:M64"/>
+    <mergeCell ref="K65:M65"/>
+    <mergeCell ref="K57:M57"/>
+    <mergeCell ref="K58:M58"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="K61:M61"/>
   </mergeCells>
-  <phoneticPr fontId="26" type="noConversion"/>
+  <phoneticPr fontId="25" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" sqref="A5:C7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>тип_детали</formula1>

</xml_diff>

<commit_message>
feat(export): add prisadka number and designer to Excel/GAS export
</commit_message>
<xml_diff>
--- a/public/templates/order_template.xlsx
+++ b/public/templates/order_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\CNC_Milling\WORK_CNC\SOFT\ProjectDB\CRM\UI_ERP\React-Admin\front_Refine_v1\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CFD1E0-8F68-44DC-B68C-9D59274D47B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97363F81-ABCC-47FD-9DCA-8AAC1803661A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="3390" windowWidth="16350" windowHeight="18210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="1635" windowWidth="17460" windowHeight="19965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заказ" sheetId="1" r:id="rId1"/>
@@ -577,15 +577,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="22"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="6"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -628,6 +619,15 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1048,10 +1048,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1060,179 +1060,179 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1545,7 +1545,7 @@
   <dimension ref="A1:AA97"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:I9"/>
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,25 +1577,25 @@
         <v>25</v>
       </c>
       <c r="B1" s="68"/>
-      <c r="C1" s="127"/>
+      <c r="C1" s="81"/>
       <c r="D1" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="93" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="86" t="s">
+      <c r="E1" s="111" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="86"/>
-      <c r="L1" s="92" t="s">
+      <c r="K1" s="115"/>
+      <c r="L1" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="92"/>
+      <c r="M1" s="110"/>
       <c r="N1" s="59"/>
       <c r="P1" s="36" t="s">
         <v>87</v>
@@ -1607,25 +1607,25 @@
     <row r="2" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="125" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="132" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="99">
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="117">
         <f>SUM(J12:J67)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="99"/>
-      <c r="L2" s="98">
+      <c r="K2" s="117"/>
+      <c r="L2" s="116">
         <f>J2-(J2*P2)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="98"/>
+      <c r="M2" s="116"/>
       <c r="N2" s="60"/>
       <c r="O2" s="37"/>
       <c r="P2" s="58"/>
@@ -1637,17 +1637,17 @@
     <row r="3" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68"/>
       <c r="B3" s="68"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
       <c r="N3" s="60"/>
       <c r="O3" s="37"/>
       <c r="P3" s="48"/>
@@ -1658,45 +1658,45 @@
       <c r="V3" s="35"/>
       <c r="W3" s="35"/>
       <c r="X3" s="35"/>
-      <c r="Y3" s="80" t="s">
+      <c r="Y3" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" s="81"/>
-      <c r="AA3" s="81"/>
+      <c r="Z3" s="127"/>
+      <c r="AA3" s="127"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="103"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="102" t="s">
+      <c r="B4" s="90"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="104"/>
-      <c r="F4" s="84" t="s">
+      <c r="E4" s="91"/>
+      <c r="F4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="95" t="s">
+      <c r="G4" s="100"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="96">
+      <c r="K4" s="113">
         <f>IF(ISBLANK(L2), (J2-SUM(Q6:Q42)), (L2-SUM(Q6:Q42)))</f>
         <v>0</v>
       </c>
-      <c r="L4" s="96"/>
-      <c r="M4" s="97"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="114"/>
       <c r="N4" s="38"/>
-      <c r="O4" s="82" t="s">
+      <c r="O4" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="82" t="s">
+      <c r="P4" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="Q4" s="100" t="s">
+      <c r="Q4" s="86" t="s">
         <v>86</v>
       </c>
       <c r="R4" s="38"/>
@@ -1706,28 +1706,28 @@
       <c r="V4" s="35"/>
       <c r="W4" s="35"/>
       <c r="X4" s="35"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="81"/>
-      <c r="AA4" s="81"/>
+      <c r="Y4" s="126"/>
+      <c r="Z4" s="127"/>
+      <c r="AA4" s="127"/>
     </row>
     <row r="5" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="113"/>
       <c r="N5" s="38"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="100"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="86"/>
       <c r="R5" s="38"/>
       <c r="S5" s="38"/>
       <c r="T5" s="38"/>
@@ -1742,21 +1742,21 @@
       <c r="Z5" s="33"/>
     </row>
     <row r="6" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="95" t="s">
+      <c r="A6" s="93"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
       <c r="N6" s="39"/>
       <c r="O6" s="62"/>
       <c r="P6" s="63"/>
@@ -1766,19 +1766,19 @@
       <c r="T6" s="39"/>
     </row>
     <row r="7" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
+      <c r="A7" s="93"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
       <c r="N7" s="39"/>
       <c r="O7" s="62"/>
       <c r="P7" s="63"/>
@@ -1788,28 +1788,28 @@
       <c r="T7" s="39"/>
     </row>
     <row r="8" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="111"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="130"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="133"/>
-      <c r="I8" s="130"/>
-      <c r="J8" s="88" t="s">
+      <c r="H8" s="122"/>
+      <c r="I8" s="123"/>
+      <c r="J8" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="121">
+      <c r="K8" s="108">
         <f>SUM(E12:E67)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="88" t="s">
+      <c r="L8" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="90">
+      <c r="M8" s="119">
         <f>SUM(D12:D67)</f>
         <v>0</v>
       </c>
@@ -1822,19 +1822,19 @@
       <c r="T8" s="14"/>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="109"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="112"/>
+      <c r="A9" s="97"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="131"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="132"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="122"/>
-      <c r="L9" s="89"/>
-      <c r="M9" s="91"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="120"/>
       <c r="N9" s="14"/>
       <c r="O9" s="64"/>
       <c r="P9" s="8"/>
@@ -1842,7 +1842,7 @@
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
-      <c r="U9" s="86" t="s">
+      <c r="U9" s="115" t="s">
         <v>80</v>
       </c>
       <c r="V9" s="1" t="s">
@@ -1871,7 +1871,7 @@
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
-      <c r="U10" s="86"/>
+      <c r="U10" s="115"/>
     </row>
     <row r="11" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -1904,11 +1904,11 @@
       <c r="J11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="87" t="s">
+      <c r="K11" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="L11" s="87"/>
-      <c r="M11" s="87"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="118"/>
       <c r="N11" s="40"/>
       <c r="O11" s="65"/>
       <c r="P11" s="66"/>
@@ -1953,9 +1953,9 @@
         <f t="shared" ref="J12:J42" si="0">E12*I12</f>
         <v>0</v>
       </c>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
       <c r="N12" s="5"/>
       <c r="O12" s="67"/>
       <c r="P12" s="8"/>
@@ -2007,9 +2007,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="87"/>
       <c r="N13" s="5"/>
       <c r="O13" s="67"/>
       <c r="P13" s="8"/>
@@ -2058,9 +2058,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="79"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="79"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="87"/>
       <c r="N14" s="5"/>
       <c r="O14" s="67"/>
       <c r="P14" s="8"/>
@@ -2109,9 +2109,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="50"/>
@@ -2160,9 +2160,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="50"/>
@@ -2211,9 +2211,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K17" s="79"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="50"/>
@@ -2262,9 +2262,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="79"/>
-      <c r="L18" s="79"/>
-      <c r="M18" s="79"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="50"/>
@@ -2313,9 +2313,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="87"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="50"/>
@@ -2364,9 +2364,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="79"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="50"/>
@@ -2415,9 +2415,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="79"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="79"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="87"/>
+      <c r="M21" s="87"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="50"/>
@@ -2466,9 +2466,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="79"/>
-      <c r="L22" s="79"/>
-      <c r="M22" s="79"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="50"/>
@@ -2517,9 +2517,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="50"/>
@@ -2568,9 +2568,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="79"/>
+      <c r="K24" s="87"/>
+      <c r="L24" s="87"/>
+      <c r="M24" s="87"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="50"/>
@@ -2619,9 +2619,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
-      <c r="M25" s="79"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="87"/>
+      <c r="M25" s="87"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="50"/>
@@ -2670,9 +2670,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="79"/>
-      <c r="L26" s="79"/>
-      <c r="M26" s="79"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="87"/>
+      <c r="M26" s="87"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="50"/>
@@ -2721,9 +2721,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="79"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="50"/>
@@ -2772,9 +2772,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="76"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="121"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="50"/>
@@ -2823,9 +2823,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="79"/>
-      <c r="L29" s="79"/>
-      <c r="M29" s="76"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="121"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="50"/>
@@ -2874,9 +2874,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="76"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="121"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="50"/>
@@ -2925,9 +2925,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K31" s="79"/>
-      <c r="L31" s="79"/>
-      <c r="M31" s="76"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="87"/>
+      <c r="M31" s="121"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="50"/>
@@ -2976,9 +2976,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K32" s="79"/>
-      <c r="L32" s="79"/>
-      <c r="M32" s="79"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
+      <c r="M32" s="87"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="50"/>
@@ -3027,9 +3027,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
-      <c r="M33" s="79"/>
+      <c r="K33" s="87"/>
+      <c r="L33" s="87"/>
+      <c r="M33" s="87"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="50"/>
@@ -3078,9 +3078,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
-      <c r="M34" s="79"/>
+      <c r="K34" s="87"/>
+      <c r="L34" s="87"/>
+      <c r="M34" s="87"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="50"/>
@@ -3129,9 +3129,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
+      <c r="K35" s="87"/>
+      <c r="L35" s="87"/>
+      <c r="M35" s="87"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="50"/>
@@ -3180,9 +3180,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K36" s="79"/>
-      <c r="L36" s="79"/>
-      <c r="M36" s="79"/>
+      <c r="K36" s="87"/>
+      <c r="L36" s="87"/>
+      <c r="M36" s="87"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="50"/>
@@ -3231,9 +3231,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
+      <c r="K37" s="87"/>
+      <c r="L37" s="87"/>
+      <c r="M37" s="87"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="50"/>
@@ -3282,9 +3282,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="79"/>
+      <c r="K38" s="87"/>
+      <c r="L38" s="87"/>
+      <c r="M38" s="87"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="50"/>
@@ -3333,9 +3333,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
+      <c r="K39" s="87"/>
+      <c r="L39" s="87"/>
+      <c r="M39" s="87"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="50"/>
@@ -3384,9 +3384,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="79"/>
+      <c r="K40" s="87"/>
+      <c r="L40" s="87"/>
+      <c r="M40" s="87"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="50"/>
@@ -3435,9 +3435,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K41" s="79"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="79"/>
+      <c r="K41" s="87"/>
+      <c r="L41" s="87"/>
+      <c r="M41" s="87"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
       <c r="P41" s="50"/>
@@ -3486,9 +3486,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K42" s="79"/>
-      <c r="L42" s="79"/>
-      <c r="M42" s="79"/>
+      <c r="K42" s="87"/>
+      <c r="L42" s="87"/>
+      <c r="M42" s="87"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="50"/>
@@ -3537,9 +3537,9 @@
         <f t="shared" ref="J43:J66" si="9">E43*I43</f>
         <v>0</v>
       </c>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="79"/>
+      <c r="K43" s="87"/>
+      <c r="L43" s="87"/>
+      <c r="M43" s="87"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="50"/>
@@ -3588,9 +3588,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K44" s="79"/>
-      <c r="L44" s="79"/>
-      <c r="M44" s="79"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="87"/>
+      <c r="M44" s="87"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="50"/>
@@ -3639,9 +3639,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="79"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="87"/>
+      <c r="M45" s="87"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="50"/>
@@ -3690,9 +3690,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K46" s="79"/>
-      <c r="L46" s="79"/>
-      <c r="M46" s="79"/>
+      <c r="K46" s="87"/>
+      <c r="L46" s="87"/>
+      <c r="M46" s="87"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="50"/>
@@ -3741,9 +3741,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K47" s="79"/>
-      <c r="L47" s="79"/>
-      <c r="M47" s="79"/>
+      <c r="K47" s="87"/>
+      <c r="L47" s="87"/>
+      <c r="M47" s="87"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="50"/>
@@ -3792,9 +3792,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K48" s="79"/>
-      <c r="L48" s="79"/>
-      <c r="M48" s="79"/>
+      <c r="K48" s="87"/>
+      <c r="L48" s="87"/>
+      <c r="M48" s="87"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="50"/>
@@ -3843,9 +3843,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K49" s="79"/>
-      <c r="L49" s="79"/>
-      <c r="M49" s="79"/>
+      <c r="K49" s="87"/>
+      <c r="L49" s="87"/>
+      <c r="M49" s="87"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="50"/>
@@ -3894,9 +3894,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K50" s="79"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="79"/>
+      <c r="K50" s="87"/>
+      <c r="L50" s="87"/>
+      <c r="M50" s="87"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="50"/>
@@ -3945,9 +3945,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K51" s="76"/>
-      <c r="L51" s="77"/>
-      <c r="M51" s="78"/>
+      <c r="K51" s="121"/>
+      <c r="L51" s="128"/>
+      <c r="M51" s="129"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="50"/>
@@ -3996,9 +3996,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K52" s="76"/>
-      <c r="L52" s="77"/>
-      <c r="M52" s="78"/>
+      <c r="K52" s="121"/>
+      <c r="L52" s="128"/>
+      <c r="M52" s="129"/>
       <c r="P52" s="50"/>
       <c r="Q52" s="52"/>
       <c r="T52" s="19"/>
@@ -4043,9 +4043,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K53" s="76"/>
-      <c r="L53" s="77"/>
-      <c r="M53" s="78"/>
+      <c r="K53" s="121"/>
+      <c r="L53" s="128"/>
+      <c r="M53" s="129"/>
       <c r="P53" s="50"/>
       <c r="Q53" s="52"/>
     </row>
@@ -4068,9 +4068,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K54" s="76"/>
-      <c r="L54" s="77"/>
-      <c r="M54" s="78"/>
+      <c r="K54" s="121"/>
+      <c r="L54" s="128"/>
+      <c r="M54" s="129"/>
       <c r="N54" s="41"/>
       <c r="O54" s="41"/>
       <c r="P54" s="53"/>
@@ -4098,9 +4098,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K55" s="76"/>
-      <c r="L55" s="77"/>
-      <c r="M55" s="78"/>
+      <c r="K55" s="121"/>
+      <c r="L55" s="128"/>
+      <c r="M55" s="129"/>
       <c r="N55" s="41"/>
       <c r="O55" s="41"/>
       <c r="P55" s="53"/>
@@ -4128,9 +4128,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K56" s="76"/>
-      <c r="L56" s="77"/>
-      <c r="M56" s="78"/>
+      <c r="K56" s="121"/>
+      <c r="L56" s="128"/>
+      <c r="M56" s="129"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" s="55"/>
@@ -4158,9 +4158,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K57" s="76"/>
-      <c r="L57" s="77"/>
-      <c r="M57" s="78"/>
+      <c r="K57" s="121"/>
+      <c r="L57" s="128"/>
+      <c r="M57" s="129"/>
       <c r="P57" s="50"/>
       <c r="Q57" s="52"/>
     </row>
@@ -4183,9 +4183,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K58" s="76"/>
-      <c r="L58" s="77"/>
-      <c r="M58" s="78"/>
+      <c r="K58" s="121"/>
+      <c r="L58" s="128"/>
+      <c r="M58" s="129"/>
     </row>
     <row r="59" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
@@ -4206,9 +4206,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K59" s="76"/>
-      <c r="L59" s="77"/>
-      <c r="M59" s="78"/>
+      <c r="K59" s="121"/>
+      <c r="L59" s="128"/>
+      <c r="M59" s="129"/>
       <c r="N59"/>
       <c r="O59"/>
       <c r="P59"/>
@@ -4241,9 +4241,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K60" s="76"/>
-      <c r="L60" s="77"/>
-      <c r="M60" s="78"/>
+      <c r="K60" s="121"/>
+      <c r="L60" s="128"/>
+      <c r="M60" s="129"/>
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60"/>
@@ -4276,9 +4276,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K61" s="76"/>
-      <c r="L61" s="77"/>
-      <c r="M61" s="78"/>
+      <c r="K61" s="121"/>
+      <c r="L61" s="128"/>
+      <c r="M61" s="129"/>
       <c r="N61"/>
       <c r="O61"/>
       <c r="P61"/>
@@ -4311,9 +4311,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K62" s="76"/>
-      <c r="L62" s="77"/>
-      <c r="M62" s="78"/>
+      <c r="K62" s="121"/>
+      <c r="L62" s="128"/>
+      <c r="M62" s="129"/>
       <c r="N62"/>
       <c r="O62"/>
       <c r="P62"/>
@@ -4346,9 +4346,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K63" s="76"/>
-      <c r="L63" s="77"/>
-      <c r="M63" s="78"/>
+      <c r="K63" s="121"/>
+      <c r="L63" s="128"/>
+      <c r="M63" s="129"/>
       <c r="N63"/>
       <c r="O63"/>
       <c r="P63"/>
@@ -4381,9 +4381,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K64" s="76"/>
-      <c r="L64" s="77"/>
-      <c r="M64" s="78"/>
+      <c r="K64" s="121"/>
+      <c r="L64" s="128"/>
+      <c r="M64" s="129"/>
       <c r="N64"/>
       <c r="O64"/>
       <c r="P64"/>
@@ -4416,9 +4416,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K65" s="76"/>
-      <c r="L65" s="77"/>
-      <c r="M65" s="78"/>
+      <c r="K65" s="121"/>
+      <c r="L65" s="128"/>
+      <c r="M65" s="129"/>
       <c r="N65"/>
       <c r="O65"/>
       <c r="P65"/>
@@ -4451,9 +4451,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K66" s="76"/>
-      <c r="L66" s="77"/>
-      <c r="M66" s="78"/>
+      <c r="K66" s="121"/>
+      <c r="L66" s="128"/>
+      <c r="M66" s="129"/>
       <c r="N66"/>
       <c r="O66"/>
       <c r="P66"/>
@@ -4482,16 +4482,16 @@
       <c r="Y67"/>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A68" s="124" t="s">
+      <c r="A68" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B68" s="124"/>
-      <c r="C68" s="124"/>
-      <c r="D68" s="124"/>
-      <c r="E68" s="124"/>
-      <c r="F68" s="124"/>
-      <c r="G68" s="124"/>
-      <c r="H68" s="124"/>
+      <c r="B68" s="80"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="80"/>
+      <c r="F68" s="80"/>
+      <c r="G68" s="80"/>
+      <c r="H68" s="80"/>
       <c r="I68" s="4" t="s">
         <v>15</v>
       </c>
@@ -4509,14 +4509,14 @@
       <c r="Y68"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A69" s="124"/>
-      <c r="B69" s="124"/>
-      <c r="C69" s="124"/>
-      <c r="D69" s="124"/>
-      <c r="E69" s="124"/>
-      <c r="F69" s="124"/>
-      <c r="G69" s="124"/>
-      <c r="H69" s="124"/>
+      <c r="A69" s="80"/>
+      <c r="B69" s="80"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="80"/>
+      <c r="F69" s="80"/>
+      <c r="G69" s="80"/>
+      <c r="H69" s="80"/>
       <c r="I69" s="3"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
@@ -4536,17 +4536,17 @@
       <c r="Y69"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A70" s="129" t="s">
+      <c r="A70" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="B70" s="129"/>
-      <c r="C70" s="129"/>
-      <c r="D70" s="129"/>
-      <c r="E70" s="129"/>
-      <c r="F70" s="129"/>
-      <c r="G70" s="129"/>
-      <c r="H70" s="129"/>
-      <c r="I70" s="129"/>
+      <c r="B70" s="83"/>
+      <c r="C70" s="83"/>
+      <c r="D70" s="83"/>
+      <c r="E70" s="83"/>
+      <c r="F70" s="83"/>
+      <c r="G70" s="83"/>
+      <c r="H70" s="83"/>
+      <c r="I70" s="83"/>
       <c r="J70" s="41"/>
       <c r="K70" s="41"/>
       <c r="L70" s="41"/>
@@ -4565,16 +4565,16 @@
       <c r="Y70"/>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A71" s="124" t="s">
+      <c r="A71" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B71" s="124"/>
-      <c r="C71" s="124"/>
-      <c r="D71" s="124"/>
-      <c r="E71" s="124"/>
-      <c r="F71" s="124"/>
-      <c r="G71" s="124"/>
-      <c r="H71" s="124"/>
+      <c r="B71" s="80"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="80"/>
+      <c r="F71" s="80"/>
+      <c r="G71" s="80"/>
+      <c r="H71" s="80"/>
       <c r="I71" s="5" t="s">
         <v>16</v>
       </c>
@@ -4596,14 +4596,14 @@
       <c r="Y71"/>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A72" s="124"/>
-      <c r="B72" s="124"/>
-      <c r="C72" s="124"/>
-      <c r="D72" s="124"/>
-      <c r="E72" s="124"/>
-      <c r="F72" s="124"/>
-      <c r="G72" s="124"/>
-      <c r="H72" s="124"/>
+      <c r="A72" s="80"/>
+      <c r="B72" s="80"/>
+      <c r="C72" s="80"/>
+      <c r="D72" s="80"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="80"/>
+      <c r="G72" s="80"/>
+      <c r="H72" s="80"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="N72"/>
@@ -5094,13 +5094,76 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="93">
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A71:H72"/>
-    <mergeCell ref="A68:H69"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="A70:I70"/>
+    <mergeCell ref="K66:M66"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="K55:M55"/>
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="K63:M63"/>
+    <mergeCell ref="K64:M64"/>
+    <mergeCell ref="K65:M65"/>
+    <mergeCell ref="K57:M57"/>
+    <mergeCell ref="K58:M58"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="Y3:AA4"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E2:I3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:M5"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="J2:K3"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="K18:M18"/>
@@ -5117,76 +5180,13 @@
     <mergeCell ref="D5:E7"/>
     <mergeCell ref="F5:G7"/>
     <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="E2:I3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:M5"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="J2:K3"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="Y3:AA4"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="K46:M46"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="K66:M66"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="K52:M52"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="K54:M54"/>
-    <mergeCell ref="K55:M55"/>
-    <mergeCell ref="K56:M56"/>
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="K63:M63"/>
-    <mergeCell ref="K64:M64"/>
-    <mergeCell ref="K65:M65"/>
-    <mergeCell ref="K57:M57"/>
-    <mergeCell ref="K58:M58"/>
-    <mergeCell ref="K59:M59"/>
-    <mergeCell ref="K60:M60"/>
-    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="A71:H72"/>
+    <mergeCell ref="A68:H69"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="A70:I70"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <dataValidations count="6">

</xml_diff>

<commit_message>
feat(analytics): add clients_analytics_view and payments_view resources
</commit_message>
<xml_diff>
--- a/public/templates/order_template.xlsx
+++ b/public/templates/order_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\CNC_Milling\WORK_CNC\SOFT\ProjectDB\CRM\UI_ERP\React-Admin\front_Refine_v1\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97363F81-ABCC-47FD-9DCA-8AAC1803661A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8E69F3-D274-40AF-8BE4-1DE9296F7167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1635" windowWidth="17460" windowHeight="19965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="2685" windowWidth="16845" windowHeight="18210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заказ" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
     <numFmt numFmtId="165" formatCode="#,##0_р_."/>
     <numFmt numFmtId="166" formatCode="#,##0\ [$KZT]"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,13 +513,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -546,30 +539,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -579,14 +548,6 @@
     <font>
       <sz val="6"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -624,6 +585,13 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -845,7 +813,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -966,12 +934,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -979,9 +941,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1009,33 +968,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1048,11 +989,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1063,175 +1001,196 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1545,7 +1504,7 @@
   <dimension ref="A1:AA97"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,91 +1525,91 @@
     <col min="14" max="14" width="1.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="46" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="44" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="3.7109375" style="1" customWidth="1"/>
     <col min="21" max="24" width="11.85546875" style="1" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69">
+      <c r="A1" s="60">
         <v>25</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="72" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="111" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="115" t="s">
+      <c r="E1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="115"/>
-      <c r="L1" s="110" t="s">
+      <c r="K1" s="81"/>
+      <c r="L1" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="110"/>
-      <c r="N1" s="59"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="56"/>
       <c r="P1" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="54" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="132" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="120" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="117">
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="94">
         <f>SUM(J12:J67)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="117"/>
-      <c r="L2" s="116">
+      <c r="K2" s="94"/>
+      <c r="L2" s="93">
         <f>J2-(J2*P2)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="116"/>
-      <c r="N2" s="60"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="57"/>
       <c r="O2" s="37"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="61"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="58"/>
       <c r="R2" s="37"/>
       <c r="S2" s="37"/>
       <c r="T2" s="37"/>
     </row>
     <row r="3" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="133"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="60"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="57"/>
       <c r="O3" s="37"/>
-      <c r="P3" s="48"/>
+      <c r="P3" s="46"/>
       <c r="R3" s="37"/>
       <c r="S3" s="37"/>
       <c r="T3" s="37"/>
@@ -1658,45 +1617,45 @@
       <c r="V3" s="35"/>
       <c r="W3" s="35"/>
       <c r="X3" s="35"/>
-      <c r="Y3" s="126" t="s">
+      <c r="Y3" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" s="127"/>
-      <c r="AA3" s="127"/>
+      <c r="Z3" s="72"/>
+      <c r="AA3" s="72"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="89" t="s">
+      <c r="B4" s="98"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="91"/>
-      <c r="F4" s="99" t="s">
+      <c r="E4" s="99"/>
+      <c r="F4" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="100"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="78" t="s">
+      <c r="G4" s="80"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="113">
+      <c r="K4" s="91">
         <f>IF(ISBLANK(L2), (J2-SUM(Q6:Q42)), (L2-SUM(Q6:Q42)))</f>
         <v>0</v>
       </c>
-      <c r="L4" s="113"/>
-      <c r="M4" s="114"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="92"/>
       <c r="N4" s="38"/>
-      <c r="O4" s="84" t="s">
+      <c r="O4" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="Q4" s="86" t="s">
+      <c r="Q4" s="95" t="s">
         <v>86</v>
       </c>
       <c r="R4" s="38"/>
@@ -1706,28 +1665,28 @@
       <c r="V4" s="35"/>
       <c r="W4" s="35"/>
       <c r="X4" s="35"/>
-      <c r="Y4" s="126"/>
-      <c r="Z4" s="127"/>
-      <c r="AA4" s="127"/>
+      <c r="Y4" s="71"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
     </row>
     <row r="5" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="113"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
       <c r="N5" s="38"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="86"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="95"/>
       <c r="R5" s="38"/>
       <c r="S5" s="38"/>
       <c r="T5" s="38"/>
@@ -1742,107 +1701,107 @@
       <c r="Z5" s="33"/>
     </row>
     <row r="6" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="78" t="s">
+      <c r="A6" s="101"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
       <c r="N6" s="39"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="73"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="125"/>
+      <c r="Q6" s="126"/>
       <c r="R6" s="39"/>
       <c r="S6" s="39"/>
       <c r="T6" s="39"/>
     </row>
     <row r="7" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="93"/>
-      <c r="B7" s="93"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
+      <c r="A7" s="101"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="115"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="96"/>
       <c r="N7" s="39"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="44"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="125"/>
+      <c r="Q7" s="126"/>
       <c r="R7" s="39"/>
       <c r="S7" s="39"/>
       <c r="T7" s="39"/>
     </row>
     <row r="8" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="130"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="106"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="122"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="94" t="s">
+      <c r="H8" s="73"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="108">
+      <c r="K8" s="116">
         <f>SUM(E12:E67)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="94" t="s">
+      <c r="L8" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="119">
+      <c r="M8" s="85">
         <f>SUM(D12:D67)</f>
         <v>0</v>
       </c>
       <c r="N8" s="14"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="45"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="127"/>
+      <c r="Q8" s="54"/>
       <c r="R8" s="14"/>
       <c r="S8" s="14"/>
       <c r="T8" s="14"/>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="97"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="131"/>
+      <c r="A9" s="104"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="107"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="125"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="120"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="117"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="86"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="45"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="127"/>
+      <c r="Q9" s="54"/>
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
-      <c r="U9" s="115" t="s">
+      <c r="U9" s="81" t="s">
         <v>80</v>
       </c>
       <c r="V9" s="1" t="s">
@@ -1865,13 +1824,13 @@
       <c r="L10" s="12"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="45"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="127"/>
+      <c r="Q10" s="54"/>
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
-      <c r="U10" s="115"/>
+      <c r="U10" s="81"/>
     </row>
     <row r="11" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -1892,10 +1851,10 @@
       <c r="F11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="70" t="s">
+      <c r="H11" s="61" t="s">
         <v>98</v>
       </c>
       <c r="I11" s="18" t="s">
@@ -1904,15 +1863,15 @@
       <c r="J11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="118" t="s">
+      <c r="K11" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
       <c r="N11" s="40"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="49"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="128"/>
+      <c r="Q11" s="129"/>
       <c r="R11" s="40"/>
       <c r="S11" s="40"/>
       <c r="T11" s="40"/>
@@ -1941,7 +1900,7 @@
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
       <c r="D12" s="42"/>
-      <c r="E12" s="74">
+      <c r="E12" s="64">
         <f>ROUNDUP((B12/1000)*(C12/1000)*D12,2)</f>
         <v>0</v>
       </c>
@@ -1953,13 +1912,13 @@
         <f t="shared" ref="J12:J42" si="0">E12*I12</f>
         <v>0</v>
       </c>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="45"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="127"/>
+      <c r="Q12" s="54"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="19">
@@ -2007,13 +1966,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="70"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="67"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="45"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="127"/>
+      <c r="Q13" s="54"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="19"/>
@@ -2058,13 +2017,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="87"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
       <c r="N14" s="5"/>
-      <c r="O14" s="67"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="45"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="127"/>
+      <c r="Q14" s="54"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="19"/>
@@ -2109,13 +2068,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="70"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="51"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="48"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="19"/>
@@ -2160,13 +2119,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="87"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="51"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="48"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="19"/>
@@ -2211,13 +2170,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-      <c r="P17" s="50"/>
-      <c r="Q17" s="51"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="48"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="19"/>
@@ -2262,13 +2221,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="51"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="48"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="19"/>
@@ -2313,13 +2272,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K19" s="87"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="51"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="48"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="19"/>
@@ -2364,13 +2323,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="87"/>
-      <c r="L20" s="87"/>
-      <c r="M20" s="87"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="51"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="48"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="19"/>
@@ -2415,13 +2374,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="87"/>
-      <c r="L21" s="87"/>
-      <c r="M21" s="87"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="70"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="51"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="48"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="19"/>
@@ -2466,13 +2425,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="87"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="87"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="70"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="51"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="48"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="19"/>
@@ -2517,13 +2476,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="51"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="48"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="19"/>
@@ -2568,13 +2527,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="70"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="51"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="48"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="19"/>
@@ -2619,13 +2578,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="70"/>
+      <c r="M25" s="70"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="51"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="48"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="19"/>
@@ -2670,13 +2629,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
-      <c r="M26" s="87"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="70"/>
+      <c r="M26" s="70"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-      <c r="P26" s="50"/>
-      <c r="Q26" s="51"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="48"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
       <c r="T26" s="19"/>
@@ -2721,13 +2680,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="70"/>
+      <c r="M27" s="70"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="51"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="48"/>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="19"/>
@@ -2772,13 +2731,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="121"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="67"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="51"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="48"/>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
       <c r="T28" s="19"/>
@@ -2823,13 +2782,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="121"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="67"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
-      <c r="P29" s="50"/>
-      <c r="Q29" s="51"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="48"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="19"/>
@@ -2874,13 +2833,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="121"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="70"/>
+      <c r="M30" s="67"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="51"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="48"/>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="19"/>
@@ -2925,13 +2884,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="121"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="67"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="51"/>
+      <c r="P31" s="47"/>
+      <c r="Q31" s="48"/>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="19"/>
@@ -2976,13 +2935,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="87"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="70"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="51"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="48"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="19"/>
@@ -3027,13 +2986,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="87"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="51"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="48"/>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="19"/>
@@ -3078,13 +3037,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K34" s="87"/>
-      <c r="L34" s="87"/>
-      <c r="M34" s="87"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="70"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="51"/>
+      <c r="P34" s="47"/>
+      <c r="Q34" s="48"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="19"/>
@@ -3129,13 +3088,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="87"/>
-      <c r="L35" s="87"/>
-      <c r="M35" s="87"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="70"/>
+      <c r="M35" s="70"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="51"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="48"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="19"/>
@@ -3180,13 +3139,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K36" s="87"/>
-      <c r="L36" s="87"/>
-      <c r="M36" s="87"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="70"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
-      <c r="P36" s="50"/>
-      <c r="Q36" s="51"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="48"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
       <c r="T36" s="19"/>
@@ -3231,13 +3190,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="87"/>
-      <c r="L37" s="87"/>
-      <c r="M37" s="87"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="70"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
-      <c r="P37" s="50"/>
-      <c r="Q37" s="51"/>
+      <c r="P37" s="47"/>
+      <c r="Q37" s="48"/>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
       <c r="T37" s="19"/>
@@ -3282,13 +3241,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K38" s="87"/>
-      <c r="L38" s="87"/>
-      <c r="M38" s="87"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="70"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="51"/>
+      <c r="P38" s="47"/>
+      <c r="Q38" s="48"/>
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
       <c r="T38" s="19"/>
@@ -3333,13 +3292,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K39" s="87"/>
-      <c r="L39" s="87"/>
-      <c r="M39" s="87"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="70"/>
+      <c r="M39" s="70"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="51"/>
+      <c r="P39" s="47"/>
+      <c r="Q39" s="48"/>
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
       <c r="T39" s="19"/>
@@ -3384,13 +3343,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K40" s="87"/>
-      <c r="L40" s="87"/>
-      <c r="M40" s="87"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="70"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="51"/>
+      <c r="P40" s="47"/>
+      <c r="Q40" s="48"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="19"/>
@@ -3435,13 +3394,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K41" s="87"/>
-      <c r="L41" s="87"/>
-      <c r="M41" s="87"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="70"/>
+      <c r="M41" s="70"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
-      <c r="P41" s="50"/>
-      <c r="Q41" s="51"/>
+      <c r="P41" s="47"/>
+      <c r="Q41" s="48"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="19"/>
@@ -3486,13 +3445,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K42" s="87"/>
-      <c r="L42" s="87"/>
-      <c r="M42" s="87"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="70"/>
+      <c r="M42" s="70"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="51"/>
+      <c r="P42" s="47"/>
+      <c r="Q42" s="48"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
       <c r="T42" s="19"/>
@@ -3537,13 +3496,13 @@
         <f t="shared" ref="J43:J66" si="9">E43*I43</f>
         <v>0</v>
       </c>
-      <c r="K43" s="87"/>
-      <c r="L43" s="87"/>
-      <c r="M43" s="87"/>
+      <c r="K43" s="70"/>
+      <c r="L43" s="70"/>
+      <c r="M43" s="70"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="51"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="48"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
       <c r="T43" s="19"/>
@@ -3588,13 +3547,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K44" s="87"/>
-      <c r="L44" s="87"/>
-      <c r="M44" s="87"/>
+      <c r="K44" s="70"/>
+      <c r="L44" s="70"/>
+      <c r="M44" s="70"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="51"/>
+      <c r="P44" s="47"/>
+      <c r="Q44" s="48"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5"/>
       <c r="T44" s="19"/>
@@ -3639,13 +3598,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K45" s="87"/>
-      <c r="L45" s="87"/>
-      <c r="M45" s="87"/>
+      <c r="K45" s="70"/>
+      <c r="L45" s="70"/>
+      <c r="M45" s="70"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
-      <c r="P45" s="50"/>
-      <c r="Q45" s="51"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="48"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
       <c r="T45" s="19"/>
@@ -3690,13 +3649,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K46" s="87"/>
-      <c r="L46" s="87"/>
-      <c r="M46" s="87"/>
+      <c r="K46" s="70"/>
+      <c r="L46" s="70"/>
+      <c r="M46" s="70"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="51"/>
+      <c r="P46" s="47"/>
+      <c r="Q46" s="48"/>
       <c r="R46" s="5"/>
       <c r="S46" s="5"/>
       <c r="T46" s="19"/>
@@ -3741,13 +3700,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K47" s="87"/>
-      <c r="L47" s="87"/>
-      <c r="M47" s="87"/>
+      <c r="K47" s="70"/>
+      <c r="L47" s="70"/>
+      <c r="M47" s="70"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
-      <c r="P47" s="50"/>
-      <c r="Q47" s="51"/>
+      <c r="P47" s="47"/>
+      <c r="Q47" s="48"/>
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
       <c r="T47" s="19"/>
@@ -3792,13 +3751,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K48" s="87"/>
-      <c r="L48" s="87"/>
-      <c r="M48" s="87"/>
+      <c r="K48" s="70"/>
+      <c r="L48" s="70"/>
+      <c r="M48" s="70"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
-      <c r="P48" s="50"/>
-      <c r="Q48" s="51"/>
+      <c r="P48" s="47"/>
+      <c r="Q48" s="48"/>
       <c r="R48" s="5"/>
       <c r="S48" s="5"/>
       <c r="T48" s="19"/>
@@ -3843,13 +3802,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K49" s="87"/>
-      <c r="L49" s="87"/>
-      <c r="M49" s="87"/>
+      <c r="K49" s="70"/>
+      <c r="L49" s="70"/>
+      <c r="M49" s="70"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
-      <c r="P49" s="50"/>
-      <c r="Q49" s="51"/>
+      <c r="P49" s="47"/>
+      <c r="Q49" s="48"/>
       <c r="R49" s="5"/>
       <c r="S49" s="5"/>
       <c r="T49" s="19"/>
@@ -3894,13 +3853,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K50" s="87"/>
-      <c r="L50" s="87"/>
-      <c r="M50" s="87"/>
+      <c r="K50" s="70"/>
+      <c r="L50" s="70"/>
+      <c r="M50" s="70"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
-      <c r="P50" s="50"/>
-      <c r="Q50" s="51"/>
+      <c r="P50" s="47"/>
+      <c r="Q50" s="48"/>
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
       <c r="T50" s="19"/>
@@ -3945,13 +3904,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K51" s="121"/>
-      <c r="L51" s="128"/>
-      <c r="M51" s="129"/>
+      <c r="K51" s="67"/>
+      <c r="L51" s="68"/>
+      <c r="M51" s="69"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
-      <c r="P51" s="50"/>
-      <c r="Q51" s="51"/>
+      <c r="P51" s="47"/>
+      <c r="Q51" s="48"/>
       <c r="R51" s="5"/>
       <c r="S51" s="5"/>
       <c r="T51" s="19"/>
@@ -3996,11 +3955,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K52" s="121"/>
-      <c r="L52" s="128"/>
-      <c r="M52" s="129"/>
-      <c r="P52" s="50"/>
-      <c r="Q52" s="52"/>
+      <c r="K52" s="67"/>
+      <c r="L52" s="68"/>
+      <c r="M52" s="69"/>
+      <c r="P52" s="47"/>
+      <c r="Q52" s="49"/>
       <c r="T52" s="19"/>
       <c r="U52" s="36">
         <f>IF(F67="выборка",(60),IF(F67="выборка-2ступени",(67),0))</f>
@@ -4043,11 +4002,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K53" s="121"/>
-      <c r="L53" s="128"/>
-      <c r="M53" s="129"/>
-      <c r="P53" s="50"/>
-      <c r="Q53" s="52"/>
+      <c r="K53" s="67"/>
+      <c r="L53" s="68"/>
+      <c r="M53" s="69"/>
+      <c r="P53" s="47"/>
+      <c r="Q53" s="49"/>
     </row>
     <row r="54" spans="1:26" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
@@ -4068,13 +4027,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K54" s="121"/>
-      <c r="L54" s="128"/>
-      <c r="M54" s="129"/>
+      <c r="K54" s="67"/>
+      <c r="L54" s="68"/>
+      <c r="M54" s="69"/>
       <c r="N54" s="41"/>
       <c r="O54" s="41"/>
-      <c r="P54" s="53"/>
-      <c r="Q54" s="54"/>
+      <c r="P54" s="50"/>
+      <c r="Q54" s="51"/>
       <c r="R54" s="41"/>
       <c r="S54" s="41"/>
       <c r="T54" s="41"/>
@@ -4098,13 +4057,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K55" s="121"/>
-      <c r="L55" s="128"/>
-      <c r="M55" s="129"/>
+      <c r="K55" s="67"/>
+      <c r="L55" s="68"/>
+      <c r="M55" s="69"/>
       <c r="N55" s="41"/>
       <c r="O55" s="41"/>
-      <c r="P55" s="53"/>
-      <c r="Q55" s="54"/>
+      <c r="P55" s="50"/>
+      <c r="Q55" s="51"/>
       <c r="R55" s="41"/>
       <c r="S55" s="41"/>
       <c r="T55" s="41"/>
@@ -4128,13 +4087,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K56" s="121"/>
-      <c r="L56" s="128"/>
-      <c r="M56" s="129"/>
+      <c r="K56" s="67"/>
+      <c r="L56" s="68"/>
+      <c r="M56" s="69"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
-      <c r="P56" s="55"/>
-      <c r="Q56" s="56"/>
+      <c r="P56" s="52"/>
+      <c r="Q56" s="53"/>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
@@ -4158,11 +4117,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K57" s="121"/>
-      <c r="L57" s="128"/>
-      <c r="M57" s="129"/>
-      <c r="P57" s="50"/>
-      <c r="Q57" s="52"/>
+      <c r="K57" s="67"/>
+      <c r="L57" s="68"/>
+      <c r="M57" s="69"/>
+      <c r="P57" s="47"/>
+      <c r="Q57" s="49"/>
     </row>
     <row r="58" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
@@ -4183,9 +4142,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K58" s="121"/>
-      <c r="L58" s="128"/>
-      <c r="M58" s="129"/>
+      <c r="K58" s="67"/>
+      <c r="L58" s="68"/>
+      <c r="M58" s="69"/>
     </row>
     <row r="59" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
@@ -4206,13 +4165,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K59" s="121"/>
-      <c r="L59" s="128"/>
-      <c r="M59" s="129"/>
+      <c r="K59" s="67"/>
+      <c r="L59" s="68"/>
+      <c r="M59" s="69"/>
       <c r="N59"/>
       <c r="O59"/>
       <c r="P59"/>
-      <c r="Q59" s="47"/>
+      <c r="Q59" s="45"/>
       <c r="R59"/>
       <c r="S59"/>
       <c r="T59"/>
@@ -4241,13 +4200,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K60" s="121"/>
-      <c r="L60" s="128"/>
-      <c r="M60" s="129"/>
+      <c r="K60" s="67"/>
+      <c r="L60" s="68"/>
+      <c r="M60" s="69"/>
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60"/>
-      <c r="Q60" s="47"/>
+      <c r="Q60" s="45"/>
       <c r="R60"/>
       <c r="S60"/>
       <c r="T60"/>
@@ -4276,13 +4235,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K61" s="121"/>
-      <c r="L61" s="128"/>
-      <c r="M61" s="129"/>
+      <c r="K61" s="67"/>
+      <c r="L61" s="68"/>
+      <c r="M61" s="69"/>
       <c r="N61"/>
       <c r="O61"/>
       <c r="P61"/>
-      <c r="Q61" s="47"/>
+      <c r="Q61" s="45"/>
       <c r="R61"/>
       <c r="S61"/>
       <c r="T61"/>
@@ -4311,13 +4270,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K62" s="121"/>
-      <c r="L62" s="128"/>
-      <c r="M62" s="129"/>
+      <c r="K62" s="67"/>
+      <c r="L62" s="68"/>
+      <c r="M62" s="69"/>
       <c r="N62"/>
       <c r="O62"/>
       <c r="P62"/>
-      <c r="Q62" s="47"/>
+      <c r="Q62" s="45"/>
       <c r="R62"/>
       <c r="S62"/>
       <c r="T62"/>
@@ -4346,13 +4305,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K63" s="121"/>
-      <c r="L63" s="128"/>
-      <c r="M63" s="129"/>
+      <c r="K63" s="67"/>
+      <c r="L63" s="68"/>
+      <c r="M63" s="69"/>
       <c r="N63"/>
       <c r="O63"/>
       <c r="P63"/>
-      <c r="Q63" s="47"/>
+      <c r="Q63" s="45"/>
       <c r="R63"/>
       <c r="S63"/>
       <c r="T63"/>
@@ -4381,13 +4340,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K64" s="121"/>
-      <c r="L64" s="128"/>
-      <c r="M64" s="129"/>
+      <c r="K64" s="67"/>
+      <c r="L64" s="68"/>
+      <c r="M64" s="69"/>
       <c r="N64"/>
       <c r="O64"/>
       <c r="P64"/>
-      <c r="Q64" s="47"/>
+      <c r="Q64" s="45"/>
       <c r="R64"/>
       <c r="S64"/>
       <c r="T64"/>
@@ -4416,13 +4375,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K65" s="121"/>
-      <c r="L65" s="128"/>
-      <c r="M65" s="129"/>
+      <c r="K65" s="67"/>
+      <c r="L65" s="68"/>
+      <c r="M65" s="69"/>
       <c r="N65"/>
       <c r="O65"/>
       <c r="P65"/>
-      <c r="Q65" s="47"/>
+      <c r="Q65" s="45"/>
       <c r="R65"/>
       <c r="S65"/>
       <c r="T65"/>
@@ -4451,13 +4410,13 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K66" s="121"/>
-      <c r="L66" s="128"/>
-      <c r="M66" s="129"/>
+      <c r="K66" s="67"/>
+      <c r="L66" s="68"/>
+      <c r="M66" s="69"/>
       <c r="N66"/>
       <c r="O66"/>
       <c r="P66"/>
-      <c r="Q66" s="47"/>
+      <c r="Q66" s="45"/>
       <c r="R66"/>
       <c r="S66"/>
       <c r="T66"/>
@@ -4471,7 +4430,7 @@
       <c r="N67"/>
       <c r="O67"/>
       <c r="P67"/>
-      <c r="Q67" s="47"/>
+      <c r="Q67" s="45"/>
       <c r="R67"/>
       <c r="S67"/>
       <c r="T67"/>
@@ -4482,23 +4441,23 @@
       <c r="Y67"/>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A68" s="80" t="s">
+      <c r="A68" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="B68" s="80"/>
-      <c r="C68" s="80"/>
-      <c r="D68" s="80"/>
-      <c r="E68" s="80"/>
-      <c r="F68" s="80"/>
-      <c r="G68" s="80"/>
-      <c r="H68" s="80"/>
+      <c r="B68" s="119"/>
+      <c r="C68" s="119"/>
+      <c r="D68" s="119"/>
+      <c r="E68" s="119"/>
+      <c r="F68" s="119"/>
+      <c r="G68" s="119"/>
+      <c r="H68" s="119"/>
       <c r="I68" s="4" t="s">
         <v>15</v>
       </c>
       <c r="N68"/>
       <c r="O68"/>
       <c r="P68"/>
-      <c r="Q68" s="47"/>
+      <c r="Q68" s="45"/>
       <c r="R68"/>
       <c r="S68"/>
       <c r="T68"/>
@@ -4509,14 +4468,14 @@
       <c r="Y68"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A69" s="80"/>
-      <c r="B69" s="80"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="80"/>
-      <c r="E69" s="80"/>
-      <c r="F69" s="80"/>
-      <c r="G69" s="80"/>
-      <c r="H69" s="80"/>
+      <c r="A69" s="119"/>
+      <c r="B69" s="119"/>
+      <c r="C69" s="119"/>
+      <c r="D69" s="119"/>
+      <c r="E69" s="119"/>
+      <c r="F69" s="119"/>
+      <c r="G69" s="119"/>
+      <c r="H69" s="119"/>
       <c r="I69" s="3"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
@@ -4525,7 +4484,7 @@
       <c r="N69"/>
       <c r="O69"/>
       <c r="P69"/>
-      <c r="Q69" s="47"/>
+      <c r="Q69" s="45"/>
       <c r="R69"/>
       <c r="S69"/>
       <c r="T69"/>
@@ -4536,17 +4495,17 @@
       <c r="Y69"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A70" s="83" t="s">
+      <c r="A70" s="124" t="s">
         <v>103</v>
       </c>
-      <c r="B70" s="83"/>
-      <c r="C70" s="83"/>
-      <c r="D70" s="83"/>
-      <c r="E70" s="83"/>
-      <c r="F70" s="83"/>
-      <c r="G70" s="83"/>
-      <c r="H70" s="83"/>
-      <c r="I70" s="83"/>
+      <c r="B70" s="124"/>
+      <c r="C70" s="124"/>
+      <c r="D70" s="124"/>
+      <c r="E70" s="124"/>
+      <c r="F70" s="124"/>
+      <c r="G70" s="124"/>
+      <c r="H70" s="124"/>
+      <c r="I70" s="124"/>
       <c r="J70" s="41"/>
       <c r="K70" s="41"/>
       <c r="L70" s="41"/>
@@ -4554,7 +4513,7 @@
       <c r="N70"/>
       <c r="O70"/>
       <c r="P70"/>
-      <c r="Q70" s="47"/>
+      <c r="Q70" s="45"/>
       <c r="R70"/>
       <c r="S70"/>
       <c r="T70"/>
@@ -4565,16 +4524,16 @@
       <c r="Y70"/>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A71" s="80" t="s">
+      <c r="A71" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="B71" s="80"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="80"/>
-      <c r="E71" s="80"/>
-      <c r="F71" s="80"/>
-      <c r="G71" s="80"/>
-      <c r="H71" s="80"/>
+      <c r="B71" s="119"/>
+      <c r="C71" s="119"/>
+      <c r="D71" s="119"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
+      <c r="G71" s="119"/>
+      <c r="H71" s="119"/>
       <c r="I71" s="5" t="s">
         <v>16</v>
       </c>
@@ -4585,7 +4544,7 @@
       <c r="N71"/>
       <c r="O71"/>
       <c r="P71"/>
-      <c r="Q71" s="47"/>
+      <c r="Q71" s="45"/>
       <c r="R71"/>
       <c r="S71"/>
       <c r="T71"/>
@@ -4596,20 +4555,20 @@
       <c r="Y71"/>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A72" s="80"/>
-      <c r="B72" s="80"/>
-      <c r="C72" s="80"/>
-      <c r="D72" s="80"/>
-      <c r="E72" s="80"/>
-      <c r="F72" s="80"/>
-      <c r="G72" s="80"/>
-      <c r="H72" s="80"/>
+      <c r="A72" s="119"/>
+      <c r="B72" s="119"/>
+      <c r="C72" s="119"/>
+      <c r="D72" s="119"/>
+      <c r="E72" s="119"/>
+      <c r="F72" s="119"/>
+      <c r="G72" s="119"/>
+      <c r="H72" s="119"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="N72"/>
       <c r="O72"/>
       <c r="P72"/>
-      <c r="Q72" s="47"/>
+      <c r="Q72" s="45"/>
       <c r="R72"/>
       <c r="S72"/>
       <c r="T72"/>
@@ -4625,7 +4584,7 @@
       <c r="N73"/>
       <c r="O73"/>
       <c r="P73"/>
-      <c r="Q73" s="47"/>
+      <c r="Q73" s="45"/>
       <c r="R73"/>
       <c r="S73"/>
       <c r="T73"/>
@@ -4652,7 +4611,7 @@
       <c r="N74"/>
       <c r="O74"/>
       <c r="P74"/>
-      <c r="Q74" s="47"/>
+      <c r="Q74" s="45"/>
       <c r="R74"/>
       <c r="S74"/>
       <c r="T74"/>
@@ -4679,7 +4638,7 @@
       <c r="N75"/>
       <c r="O75"/>
       <c r="P75"/>
-      <c r="Q75" s="47"/>
+      <c r="Q75" s="45"/>
       <c r="R75"/>
       <c r="S75"/>
       <c r="T75"/>
@@ -4706,7 +4665,7 @@
       <c r="N76"/>
       <c r="O76"/>
       <c r="P76"/>
-      <c r="Q76" s="47"/>
+      <c r="Q76" s="45"/>
       <c r="R76"/>
       <c r="S76"/>
       <c r="T76"/>
@@ -4733,7 +4692,7 @@
       <c r="N77"/>
       <c r="O77"/>
       <c r="P77"/>
-      <c r="Q77" s="47"/>
+      <c r="Q77" s="45"/>
       <c r="R77"/>
       <c r="S77"/>
       <c r="T77"/>
@@ -4760,7 +4719,7 @@
       <c r="N78"/>
       <c r="O78"/>
       <c r="P78"/>
-      <c r="Q78" s="47"/>
+      <c r="Q78" s="45"/>
       <c r="R78"/>
       <c r="S78"/>
       <c r="T78"/>
@@ -4787,7 +4746,7 @@
       <c r="N79"/>
       <c r="O79"/>
       <c r="P79"/>
-      <c r="Q79" s="47"/>
+      <c r="Q79" s="45"/>
       <c r="R79"/>
       <c r="S79"/>
       <c r="T79"/>
@@ -4814,7 +4773,7 @@
       <c r="N80"/>
       <c r="O80"/>
       <c r="P80"/>
-      <c r="Q80" s="47"/>
+      <c r="Q80" s="45"/>
       <c r="R80"/>
       <c r="S80"/>
       <c r="T80"/>
@@ -4841,7 +4800,7 @@
       <c r="N81"/>
       <c r="O81"/>
       <c r="P81"/>
-      <c r="Q81" s="47"/>
+      <c r="Q81" s="45"/>
       <c r="R81"/>
       <c r="S81"/>
       <c r="T81"/>
@@ -5094,6 +5053,83 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="93">
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="A71:H72"/>
+    <mergeCell ref="A68:H69"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="A70:I70"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K6:M7"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="D5:E7"/>
+    <mergeCell ref="F5:G7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E2:I3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:M5"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="J2:K3"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="Y3:AA4"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K47:M47"/>
     <mergeCell ref="K66:M66"/>
     <mergeCell ref="K51:M51"/>
     <mergeCell ref="K52:M52"/>
@@ -5110,85 +5146,8 @@
     <mergeCell ref="K59:M59"/>
     <mergeCell ref="K60:M60"/>
     <mergeCell ref="K61:M61"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="K46:M46"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="Y3:AA4"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="E2:I3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:M5"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="J2:K3"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K6:M7"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="D5:E7"/>
-    <mergeCell ref="F5:G7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A71:H72"/>
-    <mergeCell ref="A68:H69"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="A70:I70"/>
   </mergeCells>
-  <phoneticPr fontId="25" type="noConversion"/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" sqref="A5:C7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>тип_детали</formula1>
@@ -5239,10 +5198,10 @@
       <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="65" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="29"/>

</xml_diff>